<commit_message>
Implemented Inputfile conversion into the KISS format (buy & sell)
</commit_message>
<xml_diff>
--- a/HkwgConverter/Sample/Template_Kiss_Input.xlsx
+++ b/HkwgConverter/Sample/Template_Kiss_Input.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="120" windowWidth="28515" windowHeight="15135" activeTab="1"/>
@@ -690,12 +690,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
     <numFmt numFmtId="165" formatCode="#,##0.000\ &quot;MWh&quot;"/>
+    <numFmt numFmtId="166" formatCode="0.000;[Red]0.000"/>
+    <numFmt numFmtId="167" formatCode="0.00;[Red]0.00"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -1046,7 +1048,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1159,27 +1161,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1208,12 +1189,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1271,6 +1246,39 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1279,11 +1287,16 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
     <a:clrScheme name="Larissa">
       <a:dk1>
@@ -1357,6 +1370,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1391,6 +1405,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Larissa">
@@ -1566,12 +1581,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="39.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="26.5703125" bestFit="1" customWidth="1"/>
@@ -1579,7 +1594,7 @@
     <col min="5" max="5" width="26.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1594,7 +1609,7 @@
       </c>
       <c r="E1" s="8"/>
     </row>
-    <row r="2" spans="1:5" ht="13.5" thickBot="1">
+    <row r="2" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="6" t="s">
         <v>2</v>
@@ -1607,13 +1622,13 @@
       </c>
       <c r="E2" s="9"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B6" s="10"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" s="11"/>
     </row>
   </sheetData>
@@ -1623,22 +1638,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.5703125" customWidth="1"/>
     <col min="3" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A1" s="49" t="s">
+    <row r="1" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="42" t="s">
         <v>205</v>
       </c>
       <c r="B1" s="26" t="s">
@@ -1652,7 +1667,7 @@
       </c>
       <c r="E1" s="12"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
         <v>206</v>
       </c>
@@ -1667,7 +1682,7 @@
       </c>
       <c r="E2" s="13"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="17"/>
       <c r="B3" s="16" t="s">
         <v>209</v>
@@ -1680,7 +1695,7 @@
       </c>
       <c r="E3" s="13"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="17"/>
       <c r="B4" s="18" t="s">
         <v>210</v>
@@ -1693,7 +1708,7 @@
       </c>
       <c r="E4" s="14"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="17"/>
       <c r="B5" s="18" t="s">
         <v>211</v>
@@ -1706,14 +1721,14 @@
       </c>
       <c r="E5" s="14"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="17"/>
       <c r="B6" s="19"/>
       <c r="C6" s="37"/>
       <c r="D6" s="37"/>
       <c r="E6" s="14"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="17"/>
       <c r="B7" s="18" t="s">
         <v>4</v>
@@ -1726,7 +1741,7 @@
       </c>
       <c r="E7" s="14"/>
     </row>
-    <row r="8" spans="1:5" ht="13.5" thickBot="1">
+    <row r="8" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="29"/>
       <c r="B8" s="30" t="s">
         <v>212</v>
@@ -1735,8 +1750,8 @@
       <c r="D8" s="38"/>
       <c r="E8" s="13"/>
     </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="50" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="43" t="s">
         <v>213</v>
       </c>
       <c r="B9" s="20" t="s">
@@ -1750,8 +1765,8 @@
       </c>
       <c r="E9" s="12"/>
     </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="51"/>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="44"/>
       <c r="B10" s="20" t="s">
         <v>217</v>
       </c>
@@ -1763,8 +1778,8 @@
       </c>
       <c r="E10" s="12"/>
     </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="51"/>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="44"/>
       <c r="B11" s="20" t="s">
         <v>216</v>
       </c>
@@ -1776,8 +1791,8 @@
       </c>
       <c r="E11" s="12"/>
     </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="51"/>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="44"/>
       <c r="B12" s="20" t="s">
         <v>217</v>
       </c>
@@ -1785,42 +1800,42 @@
       <c r="D12" s="39"/>
       <c r="E12" s="12"/>
     </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="51"/>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="44"/>
       <c r="B13" s="21"/>
       <c r="C13" s="39"/>
       <c r="D13" s="39"/>
       <c r="E13" s="12"/>
     </row>
-    <row r="14" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A14" s="51"/>
+    <row r="14" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="44"/>
       <c r="B14" s="21"/>
       <c r="C14" s="39"/>
       <c r="D14" s="39"/>
       <c r="E14" s="12"/>
     </row>
-    <row r="15" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A15" s="52" t="s">
+    <row r="15" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="45" t="s">
         <v>214</v>
       </c>
       <c r="B15" s="31" t="s">
         <v>218</v>
       </c>
-      <c r="C15" s="40">
-        <v>36</v>
+      <c r="C15" s="85">
+        <v>0</v>
       </c>
       <c r="D15" s="40"/>
       <c r="E15" s="12"/>
     </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="53"/>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="46"/>
       <c r="B16" s="22"/>
       <c r="C16" s="41"/>
       <c r="D16" s="41"/>
       <c r="E16" s="12"/>
     </row>
-    <row r="17" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A17" s="54" t="s">
+    <row r="17" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="47" t="s">
         <v>219</v>
       </c>
       <c r="B17" s="23" t="s">
@@ -1834,2462 +1849,2463 @@
       </c>
       <c r="E17" s="12"/>
     </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="80">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="71">
         <v>42767</v>
       </c>
       <c r="B18" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="42">
-        <v>0</v>
-      </c>
-      <c r="D18" s="46">
+      <c r="C18" s="75">
+        <v>0</v>
+      </c>
+      <c r="D18" s="80">
         <v>0</v>
       </c>
       <c r="E18" s="12"/>
     </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="81">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="72">
         <v>42767.010416666664</v>
       </c>
       <c r="B19" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="43">
-        <v>0</v>
-      </c>
-      <c r="D19" s="47">
+      <c r="C19" s="76">
+        <v>0</v>
+      </c>
+      <c r="D19" s="81">
         <v>0</v>
       </c>
       <c r="E19" s="12"/>
     </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="81">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="72">
         <v>42767.020833333336</v>
       </c>
       <c r="B20" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="43">
-        <v>0</v>
-      </c>
-      <c r="D20" s="47">
+      <c r="C20" s="76">
+        <v>0</v>
+      </c>
+      <c r="D20" s="81">
         <v>0</v>
       </c>
       <c r="E20" s="12"/>
     </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="82">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="73">
         <v>42767.03125</v>
       </c>
-      <c r="B21" s="60" t="s">
+      <c r="B21" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="61">
-        <v>0</v>
-      </c>
-      <c r="D21" s="62">
+      <c r="C21" s="77">
+        <v>0</v>
+      </c>
+      <c r="D21" s="82">
         <v>0</v>
       </c>
       <c r="E21" s="12"/>
     </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="81">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="72">
         <v>42767.041666666664</v>
       </c>
       <c r="B22" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="43">
-        <v>0</v>
-      </c>
-      <c r="D22" s="47">
+      <c r="C22" s="76">
+        <v>0</v>
+      </c>
+      <c r="D22" s="81">
         <v>0</v>
       </c>
       <c r="E22" s="12"/>
     </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="81">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="72">
         <v>42767.052083333336</v>
       </c>
       <c r="B23" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="43">
-        <v>0</v>
-      </c>
-      <c r="D23" s="47">
+      <c r="C23" s="76">
+        <v>0</v>
+      </c>
+      <c r="D23" s="81">
         <v>0</v>
       </c>
       <c r="E23" s="12"/>
     </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="81">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="72">
         <v>42767.0625</v>
       </c>
       <c r="B24" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="43">
-        <v>0</v>
-      </c>
-      <c r="D24" s="47">
+      <c r="C24" s="76">
+        <v>0</v>
+      </c>
+      <c r="D24" s="81">
         <v>0</v>
       </c>
       <c r="E24" s="12"/>
     </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="82">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="73">
         <v>42767.072916666664</v>
       </c>
-      <c r="B25" s="60" t="s">
+      <c r="B25" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="61">
-        <v>0</v>
-      </c>
-      <c r="D25" s="62">
+      <c r="C25" s="77">
+        <v>0</v>
+      </c>
+      <c r="D25" s="82">
         <v>0</v>
       </c>
       <c r="E25" s="12"/>
     </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="81">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="72">
         <v>42767.083333333336</v>
       </c>
       <c r="B26" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="43">
-        <v>0</v>
-      </c>
-      <c r="D26" s="47">
+      <c r="C26" s="76">
+        <v>0</v>
+      </c>
+      <c r="D26" s="81">
         <v>0</v>
       </c>
       <c r="E26" s="12"/>
     </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="81">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="72">
         <v>42767.09375</v>
       </c>
       <c r="B27" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="43">
-        <v>0</v>
-      </c>
-      <c r="D27" s="47">
+      <c r="C27" s="76">
+        <v>0</v>
+      </c>
+      <c r="D27" s="81">
         <v>0</v>
       </c>
       <c r="E27" s="12"/>
     </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="81">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="72">
         <v>42767.104166666664</v>
       </c>
       <c r="B28" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="C28" s="43">
-        <v>0</v>
-      </c>
-      <c r="D28" s="47">
+      <c r="C28" s="76">
+        <v>0</v>
+      </c>
+      <c r="D28" s="81">
         <v>0</v>
       </c>
       <c r="E28" s="12"/>
     </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="82">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="73">
         <v>42767.114583333336</v>
       </c>
-      <c r="B29" s="60" t="s">
+      <c r="B29" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="C29" s="61">
-        <v>0</v>
-      </c>
-      <c r="D29" s="62">
+      <c r="C29" s="77">
+        <v>0</v>
+      </c>
+      <c r="D29" s="82">
         <v>0</v>
       </c>
       <c r="E29" s="12"/>
     </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="81">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="72">
         <v>42767.125</v>
       </c>
       <c r="B30" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="43">
-        <v>0</v>
-      </c>
-      <c r="D30" s="47">
+      <c r="C30" s="76">
+        <v>0</v>
+      </c>
+      <c r="D30" s="81">
         <v>0</v>
       </c>
       <c r="E30" s="12"/>
     </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="81">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="72">
         <v>42767.135416666664</v>
       </c>
       <c r="B31" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="C31" s="43">
-        <v>0</v>
-      </c>
-      <c r="D31" s="47">
+      <c r="C31" s="76">
+        <v>0</v>
+      </c>
+      <c r="D31" s="81">
         <v>0</v>
       </c>
       <c r="E31" s="12"/>
     </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="81">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="72">
         <v>42767.145833333336</v>
       </c>
       <c r="B32" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="C32" s="43">
-        <v>0</v>
-      </c>
-      <c r="D32" s="47">
+      <c r="C32" s="76">
+        <v>0</v>
+      </c>
+      <c r="D32" s="81">
         <v>0</v>
       </c>
       <c r="E32" s="12"/>
     </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="82">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="73">
         <v>42767.15625</v>
       </c>
-      <c r="B33" s="60" t="s">
+      <c r="B33" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="C33" s="61">
-        <v>0</v>
-      </c>
-      <c r="D33" s="62">
+      <c r="C33" s="77">
+        <v>0</v>
+      </c>
+      <c r="D33" s="82">
         <v>0</v>
       </c>
       <c r="E33" s="12"/>
     </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="81">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="72">
         <v>42767.166666666664</v>
       </c>
       <c r="B34" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="C34" s="43">
-        <v>0</v>
-      </c>
-      <c r="D34" s="47">
+      <c r="C34" s="76">
+        <v>0</v>
+      </c>
+      <c r="D34" s="81">
         <v>0</v>
       </c>
       <c r="E34" s="12"/>
     </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="81">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="72">
         <v>42767.177083333336</v>
       </c>
       <c r="B35" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="C35" s="43">
-        <v>0</v>
-      </c>
-      <c r="D35" s="47">
+      <c r="C35" s="76">
+        <v>0</v>
+      </c>
+      <c r="D35" s="81">
         <v>0</v>
       </c>
       <c r="E35" s="12"/>
     </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="81">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="72">
         <v>42767.1875</v>
       </c>
       <c r="B36" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="C36" s="43">
-        <v>0</v>
-      </c>
-      <c r="D36" s="47">
+      <c r="C36" s="76">
+        <v>0</v>
+      </c>
+      <c r="D36" s="81">
         <v>0</v>
       </c>
       <c r="E36" s="12"/>
     </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="82">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="73">
         <v>42767.197916666664</v>
       </c>
-      <c r="B37" s="60" t="s">
+      <c r="B37" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="C37" s="61">
-        <v>0</v>
-      </c>
-      <c r="D37" s="62">
+      <c r="C37" s="77">
+        <v>0</v>
+      </c>
+      <c r="D37" s="82">
         <v>0</v>
       </c>
       <c r="E37" s="12"/>
     </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="81">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="72">
         <v>42767.208333333336</v>
       </c>
       <c r="B38" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="C38" s="43">
-        <v>0</v>
-      </c>
-      <c r="D38" s="47">
+      <c r="C38" s="76">
+        <v>0</v>
+      </c>
+      <c r="D38" s="81">
         <v>0</v>
       </c>
       <c r="E38" s="12"/>
     </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="81">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="72">
         <v>42767.21875</v>
       </c>
       <c r="B39" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="C39" s="43">
-        <v>0</v>
-      </c>
-      <c r="D39" s="47">
+      <c r="C39" s="76">
+        <v>0</v>
+      </c>
+      <c r="D39" s="81">
         <v>0</v>
       </c>
       <c r="E39" s="12"/>
     </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="81">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="72">
         <v>42767.229166666664</v>
       </c>
       <c r="B40" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="C40" s="43">
-        <v>0</v>
-      </c>
-      <c r="D40" s="47">
+      <c r="C40" s="76">
+        <v>0</v>
+      </c>
+      <c r="D40" s="81">
         <v>0</v>
       </c>
       <c r="E40" s="12"/>
     </row>
-    <row r="41" spans="1:5">
-      <c r="A41" s="82">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="73">
         <v>42767.239583333336</v>
       </c>
-      <c r="B41" s="60" t="s">
+      <c r="B41" s="53" t="s">
         <v>55</v>
       </c>
-      <c r="C41" s="61">
-        <v>0</v>
-      </c>
-      <c r="D41" s="62">
+      <c r="C41" s="77">
+        <v>0</v>
+      </c>
+      <c r="D41" s="82">
         <v>0</v>
       </c>
       <c r="E41" s="12"/>
     </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="81">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="72">
         <v>42767.25</v>
       </c>
       <c r="B42" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="C42" s="43">
-        <v>0</v>
-      </c>
-      <c r="D42" s="47">
+      <c r="C42" s="76">
+        <v>0</v>
+      </c>
+      <c r="D42" s="81">
         <v>0</v>
       </c>
       <c r="E42" s="12"/>
     </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="81">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="72">
         <v>42767.260416666664</v>
       </c>
       <c r="B43" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="43">
-        <v>0</v>
-      </c>
-      <c r="D43" s="47">
+      <c r="C43" s="76">
+        <v>0</v>
+      </c>
+      <c r="D43" s="81">
         <v>0</v>
       </c>
       <c r="E43" s="12"/>
     </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="81">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="72">
         <v>42767.270833333336</v>
       </c>
       <c r="B44" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="C44" s="43">
-        <v>0</v>
-      </c>
-      <c r="D44" s="47">
+      <c r="C44" s="76">
+        <v>0</v>
+      </c>
+      <c r="D44" s="81">
         <v>0</v>
       </c>
       <c r="E44" s="12"/>
     </row>
-    <row r="45" spans="1:5">
-      <c r="A45" s="82">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="73">
         <v>42767.28125</v>
       </c>
-      <c r="B45" s="60" t="s">
+      <c r="B45" s="53" t="s">
         <v>63</v>
       </c>
-      <c r="C45" s="61">
-        <v>0</v>
-      </c>
-      <c r="D45" s="62">
+      <c r="C45" s="77">
+        <v>0</v>
+      </c>
+      <c r="D45" s="82">
         <v>0</v>
       </c>
       <c r="E45" s="12"/>
     </row>
-    <row r="46" spans="1:5">
-      <c r="A46" s="81">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="72">
         <v>42767.291666666664</v>
       </c>
       <c r="B46" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="C46" s="43">
-        <v>0</v>
-      </c>
-      <c r="D46" s="47">
+      <c r="C46" s="76">
+        <v>0</v>
+      </c>
+      <c r="D46" s="81">
         <v>0</v>
       </c>
       <c r="E46" s="12"/>
     </row>
-    <row r="47" spans="1:5">
-      <c r="A47" s="81">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="72">
         <v>42767.302083333336</v>
       </c>
       <c r="B47" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="C47" s="43">
-        <v>0</v>
-      </c>
-      <c r="D47" s="47">
+      <c r="C47" s="76">
+        <v>0</v>
+      </c>
+      <c r="D47" s="81">
         <v>0</v>
       </c>
       <c r="E47" s="12"/>
     </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="81">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="72">
         <v>42767.3125</v>
       </c>
       <c r="B48" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="C48" s="43">
-        <v>0</v>
-      </c>
-      <c r="D48" s="47">
+      <c r="C48" s="76">
+        <v>0</v>
+      </c>
+      <c r="D48" s="81">
         <v>0</v>
       </c>
       <c r="E48" s="12"/>
     </row>
-    <row r="49" spans="1:5">
-      <c r="A49" s="82">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="73">
         <v>42767.322916666664</v>
       </c>
-      <c r="B49" s="60" t="s">
+      <c r="B49" s="53" t="s">
         <v>71</v>
       </c>
-      <c r="C49" s="61">
-        <v>0</v>
-      </c>
-      <c r="D49" s="62">
+      <c r="C49" s="77">
+        <v>0</v>
+      </c>
+      <c r="D49" s="82">
         <v>0</v>
       </c>
       <c r="E49" s="12"/>
     </row>
-    <row r="50" spans="1:5">
-      <c r="A50" s="81">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="72">
         <v>42767.333333333336</v>
       </c>
       <c r="B50" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="C50" s="43">
-        <v>0</v>
-      </c>
-      <c r="D50" s="47">
+      <c r="C50" s="76">
+        <v>0</v>
+      </c>
+      <c r="D50" s="81">
         <v>0</v>
       </c>
       <c r="E50" s="12"/>
     </row>
-    <row r="51" spans="1:5">
-      <c r="A51" s="81">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" s="72">
         <v>42767.34375</v>
       </c>
       <c r="B51" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="C51" s="43">
-        <v>0</v>
-      </c>
-      <c r="D51" s="47">
+      <c r="C51" s="76">
+        <v>0</v>
+      </c>
+      <c r="D51" s="81">
         <v>0</v>
       </c>
       <c r="E51" s="12"/>
     </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="81">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" s="72">
         <v>42767.354166666664</v>
       </c>
       <c r="B52" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="C52" s="43">
-        <v>0</v>
-      </c>
-      <c r="D52" s="47">
+      <c r="C52" s="76">
+        <v>0</v>
+      </c>
+      <c r="D52" s="81">
         <v>0</v>
       </c>
       <c r="E52" s="12"/>
     </row>
-    <row r="53" spans="1:5">
-      <c r="A53" s="82">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" s="73">
         <v>42767.364583333336</v>
       </c>
-      <c r="B53" s="60" t="s">
+      <c r="B53" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="C53" s="61">
-        <v>0</v>
-      </c>
-      <c r="D53" s="62">
+      <c r="C53" s="77">
+        <v>0</v>
+      </c>
+      <c r="D53" s="82">
         <v>0</v>
       </c>
       <c r="E53" s="12"/>
     </row>
-    <row r="54" spans="1:5">
-      <c r="A54" s="81">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" s="72">
         <v>42767.375</v>
       </c>
       <c r="B54" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="C54" s="43">
-        <v>0</v>
-      </c>
-      <c r="D54" s="47">
+      <c r="C54" s="76">
+        <v>0</v>
+      </c>
+      <c r="D54" s="81">
         <v>0</v>
       </c>
       <c r="E54" s="12"/>
     </row>
-    <row r="55" spans="1:5">
-      <c r="A55" s="81">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" s="72">
         <v>42767.385416666664</v>
       </c>
       <c r="B55" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="C55" s="43">
-        <v>0</v>
-      </c>
-      <c r="D55" s="47">
+      <c r="C55" s="76">
+        <v>0</v>
+      </c>
+      <c r="D55" s="81">
         <v>0</v>
       </c>
       <c r="E55" s="12"/>
     </row>
-    <row r="56" spans="1:5">
-      <c r="A56" s="81">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" s="72">
         <v>42767.395833333336</v>
       </c>
       <c r="B56" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="C56" s="43">
-        <v>0</v>
-      </c>
-      <c r="D56" s="47">
+      <c r="C56" s="76">
+        <v>0</v>
+      </c>
+      <c r="D56" s="81">
         <v>0</v>
       </c>
       <c r="E56" s="12"/>
     </row>
-    <row r="57" spans="1:5">
-      <c r="A57" s="82">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" s="73">
         <v>42767.40625</v>
       </c>
-      <c r="B57" s="60" t="s">
+      <c r="B57" s="53" t="s">
         <v>87</v>
       </c>
-      <c r="C57" s="61">
-        <v>0</v>
-      </c>
-      <c r="D57" s="62">
+      <c r="C57" s="77">
+        <v>0</v>
+      </c>
+      <c r="D57" s="82">
         <v>0</v>
       </c>
       <c r="E57" s="12"/>
     </row>
-    <row r="58" spans="1:5">
-      <c r="A58" s="81">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" s="72">
         <v>42767.416666666664</v>
       </c>
       <c r="B58" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="C58" s="43">
-        <v>0</v>
-      </c>
-      <c r="D58" s="47">
+      <c r="C58" s="76">
+        <v>0</v>
+      </c>
+      <c r="D58" s="81">
         <v>0</v>
       </c>
       <c r="E58" s="12"/>
     </row>
-    <row r="59" spans="1:5">
-      <c r="A59" s="81">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" s="72">
         <v>42767.427083333336</v>
       </c>
       <c r="B59" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="C59" s="43">
-        <v>0</v>
-      </c>
-      <c r="D59" s="47">
+      <c r="C59" s="76">
+        <v>0</v>
+      </c>
+      <c r="D59" s="81">
         <v>0</v>
       </c>
       <c r="E59" s="12"/>
     </row>
-    <row r="60" spans="1:5">
-      <c r="A60" s="81">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" s="72">
         <v>42767.4375</v>
       </c>
       <c r="B60" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="C60" s="43">
-        <v>0</v>
-      </c>
-      <c r="D60" s="47">
+      <c r="C60" s="76">
+        <v>0</v>
+      </c>
+      <c r="D60" s="81">
         <v>0</v>
       </c>
       <c r="E60" s="12"/>
     </row>
-    <row r="61" spans="1:5">
-      <c r="A61" s="82">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" s="73">
         <v>42767.447916666664</v>
       </c>
-      <c r="B61" s="60" t="s">
+      <c r="B61" s="53" t="s">
         <v>95</v>
       </c>
-      <c r="C61" s="61">
-        <v>0</v>
-      </c>
-      <c r="D61" s="62">
+      <c r="C61" s="77">
+        <v>0</v>
+      </c>
+      <c r="D61" s="82">
         <v>0</v>
       </c>
       <c r="E61" s="12"/>
     </row>
-    <row r="62" spans="1:5">
-      <c r="A62" s="81">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" s="72">
         <v>42767.458333333336</v>
       </c>
       <c r="B62" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="C62" s="43">
-        <v>0</v>
-      </c>
-      <c r="D62" s="47">
+      <c r="C62" s="76">
+        <v>0</v>
+      </c>
+      <c r="D62" s="81">
         <v>0</v>
       </c>
       <c r="E62" s="12"/>
     </row>
-    <row r="63" spans="1:5">
-      <c r="A63" s="81">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" s="72">
         <v>42767.46875</v>
       </c>
       <c r="B63" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="C63" s="43">
-        <v>0</v>
-      </c>
-      <c r="D63" s="47">
+      <c r="C63" s="76">
+        <v>0</v>
+      </c>
+      <c r="D63" s="81">
         <v>0</v>
       </c>
       <c r="E63" s="12"/>
     </row>
-    <row r="64" spans="1:5">
-      <c r="A64" s="81">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" s="72">
         <v>42767.479166666664</v>
       </c>
       <c r="B64" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="C64" s="43">
-        <v>0</v>
-      </c>
-      <c r="D64" s="47">
+      <c r="C64" s="76">
+        <v>0</v>
+      </c>
+      <c r="D64" s="81">
         <v>0</v>
       </c>
       <c r="E64" s="12"/>
     </row>
-    <row r="65" spans="1:5">
-      <c r="A65" s="82">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" s="73">
         <v>42767.489583333336</v>
       </c>
-      <c r="B65" s="60" t="s">
+      <c r="B65" s="53" t="s">
         <v>103</v>
       </c>
-      <c r="C65" s="61">
-        <v>0</v>
-      </c>
-      <c r="D65" s="62">
+      <c r="C65" s="77">
+        <v>0</v>
+      </c>
+      <c r="D65" s="82">
         <v>0</v>
       </c>
       <c r="E65" s="12"/>
     </row>
-    <row r="66" spans="1:5">
-      <c r="A66" s="81">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" s="72">
         <v>42767.5</v>
       </c>
       <c r="B66" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="C66" s="43">
-        <v>0</v>
-      </c>
-      <c r="D66" s="47">
+      <c r="C66" s="76">
+        <v>0</v>
+      </c>
+      <c r="D66" s="81">
         <v>0</v>
       </c>
       <c r="E66" s="12"/>
     </row>
-    <row r="67" spans="1:5">
-      <c r="A67" s="81">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" s="72">
         <v>42767.510416666664</v>
       </c>
       <c r="B67" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="C67" s="43">
-        <v>0</v>
-      </c>
-      <c r="D67" s="47">
+      <c r="C67" s="76">
+        <v>0</v>
+      </c>
+      <c r="D67" s="81">
         <v>0</v>
       </c>
       <c r="E67" s="12"/>
     </row>
-    <row r="68" spans="1:5">
-      <c r="A68" s="81">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" s="72">
         <v>42767.520833333336</v>
       </c>
       <c r="B68" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="C68" s="43">
-        <v>0</v>
-      </c>
-      <c r="D68" s="47">
+      <c r="C68" s="76">
+        <v>0</v>
+      </c>
+      <c r="D68" s="81">
         <v>0</v>
       </c>
       <c r="E68" s="12"/>
     </row>
-    <row r="69" spans="1:5">
-      <c r="A69" s="82">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69" s="73">
         <v>42767.53125</v>
       </c>
-      <c r="B69" s="60" t="s">
+      <c r="B69" s="53" t="s">
         <v>111</v>
       </c>
-      <c r="C69" s="61">
-        <v>0</v>
-      </c>
-      <c r="D69" s="62">
+      <c r="C69" s="77">
+        <v>0</v>
+      </c>
+      <c r="D69" s="82">
         <v>0</v>
       </c>
       <c r="E69" s="12"/>
     </row>
-    <row r="70" spans="1:5">
-      <c r="A70" s="81">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70" s="72">
         <v>42767.541666666664</v>
       </c>
       <c r="B70" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="C70" s="43">
-        <v>0</v>
-      </c>
-      <c r="D70" s="47">
+      <c r="C70" s="76">
+        <v>0</v>
+      </c>
+      <c r="D70" s="81">
         <v>0</v>
       </c>
       <c r="E70" s="12"/>
     </row>
-    <row r="71" spans="1:5">
-      <c r="A71" s="81">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71" s="72">
         <v>42767.552083333336</v>
       </c>
       <c r="B71" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="C71" s="43">
-        <v>0</v>
-      </c>
-      <c r="D71" s="47">
+      <c r="C71" s="76">
+        <v>0</v>
+      </c>
+      <c r="D71" s="81">
         <v>0</v>
       </c>
       <c r="E71" s="12"/>
     </row>
-    <row r="72" spans="1:5">
-      <c r="A72" s="81">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72" s="72">
         <v>42767.5625</v>
       </c>
       <c r="B72" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="C72" s="43">
-        <v>0</v>
-      </c>
-      <c r="D72" s="47">
+      <c r="C72" s="76">
+        <v>0</v>
+      </c>
+      <c r="D72" s="81">
         <v>0</v>
       </c>
       <c r="E72" s="12"/>
     </row>
-    <row r="73" spans="1:5">
-      <c r="A73" s="82">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A73" s="73">
         <v>42767.572916666664</v>
       </c>
-      <c r="B73" s="60" t="s">
+      <c r="B73" s="53" t="s">
         <v>119</v>
       </c>
-      <c r="C73" s="61">
-        <v>0</v>
-      </c>
-      <c r="D73" s="62">
+      <c r="C73" s="77">
+        <v>0</v>
+      </c>
+      <c r="D73" s="82">
         <v>0</v>
       </c>
       <c r="E73" s="12"/>
     </row>
-    <row r="74" spans="1:5">
-      <c r="A74" s="81">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A74" s="72">
         <v>42767.583333333336</v>
       </c>
       <c r="B74" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="C74" s="43">
-        <v>0</v>
-      </c>
-      <c r="D74" s="47">
+      <c r="C74" s="76">
+        <v>0</v>
+      </c>
+      <c r="D74" s="81">
         <v>0</v>
       </c>
       <c r="E74" s="12"/>
     </row>
-    <row r="75" spans="1:5">
-      <c r="A75" s="81">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A75" s="72">
         <v>42767.59375</v>
       </c>
       <c r="B75" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="C75" s="43">
-        <v>0</v>
-      </c>
-      <c r="D75" s="47">
+      <c r="C75" s="76">
+        <v>0</v>
+      </c>
+      <c r="D75" s="81">
         <v>0</v>
       </c>
       <c r="E75" s="12"/>
     </row>
-    <row r="76" spans="1:5">
-      <c r="A76" s="81">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A76" s="72">
         <v>42767.604166666664</v>
       </c>
       <c r="B76" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="C76" s="43">
-        <v>0</v>
-      </c>
-      <c r="D76" s="47">
+      <c r="C76" s="76">
+        <v>0</v>
+      </c>
+      <c r="D76" s="81">
         <v>0</v>
       </c>
       <c r="E76" s="12"/>
     </row>
-    <row r="77" spans="1:5">
-      <c r="A77" s="82">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A77" s="73">
         <v>42767.614583333336</v>
       </c>
-      <c r="B77" s="60" t="s">
+      <c r="B77" s="53" t="s">
         <v>127</v>
       </c>
-      <c r="C77" s="61">
-        <v>0</v>
-      </c>
-      <c r="D77" s="62">
+      <c r="C77" s="77">
+        <v>0</v>
+      </c>
+      <c r="D77" s="82">
         <v>0</v>
       </c>
       <c r="E77" s="12"/>
     </row>
-    <row r="78" spans="1:5">
-      <c r="A78" s="81">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A78" s="72">
         <v>42767.625</v>
       </c>
       <c r="B78" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="C78" s="43">
-        <v>0</v>
-      </c>
-      <c r="D78" s="47">
+      <c r="C78" s="76">
+        <v>0</v>
+      </c>
+      <c r="D78" s="81">
         <v>0</v>
       </c>
       <c r="E78" s="12"/>
     </row>
-    <row r="79" spans="1:5">
-      <c r="A79" s="81">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A79" s="72">
         <v>42767.635416666664</v>
       </c>
       <c r="B79" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="C79" s="43">
-        <v>0</v>
-      </c>
-      <c r="D79" s="47">
+      <c r="C79" s="76">
+        <v>0</v>
+      </c>
+      <c r="D79" s="81">
         <v>0</v>
       </c>
       <c r="E79" s="12"/>
     </row>
-    <row r="80" spans="1:5">
-      <c r="A80" s="81">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A80" s="72">
         <v>42767.645833333336</v>
       </c>
       <c r="B80" s="24" t="s">
         <v>133</v>
       </c>
-      <c r="C80" s="43">
-        <v>0</v>
-      </c>
-      <c r="D80" s="47">
+      <c r="C80" s="76">
+        <v>0</v>
+      </c>
+      <c r="D80" s="81">
         <v>0</v>
       </c>
       <c r="E80" s="12"/>
     </row>
-    <row r="81" spans="1:5">
-      <c r="A81" s="82">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A81" s="73">
         <v>42767.65625</v>
       </c>
-      <c r="B81" s="60" t="s">
+      <c r="B81" s="53" t="s">
         <v>135</v>
       </c>
-      <c r="C81" s="61">
-        <v>0</v>
-      </c>
-      <c r="D81" s="62">
+      <c r="C81" s="77">
+        <v>0</v>
+      </c>
+      <c r="D81" s="81">
         <v>0</v>
       </c>
       <c r="E81" s="12"/>
     </row>
-    <row r="82" spans="1:5">
-      <c r="A82" s="81">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A82" s="72">
         <v>42767.666666666664</v>
       </c>
       <c r="B82" s="24" t="s">
         <v>137</v>
       </c>
-      <c r="C82" s="43">
-        <v>12</v>
-      </c>
-      <c r="D82" s="47">
-        <v>85</v>
+      <c r="C82" s="76">
+        <v>0</v>
+      </c>
+      <c r="D82" s="82">
+        <v>0</v>
       </c>
       <c r="E82" s="12"/>
     </row>
-    <row r="83" spans="1:5">
-      <c r="A83" s="81">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A83" s="72">
         <v>42767.677083333336</v>
       </c>
       <c r="B83" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="C83" s="43">
-        <v>12</v>
-      </c>
-      <c r="D83" s="47">
-        <v>85</v>
+      <c r="C83" s="76">
+        <v>0</v>
+      </c>
+      <c r="D83" s="81">
+        <v>0</v>
       </c>
       <c r="E83" s="12"/>
     </row>
-    <row r="84" spans="1:5">
-      <c r="A84" s="81">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A84" s="72">
         <v>42767.6875</v>
       </c>
       <c r="B84" s="24" t="s">
         <v>141</v>
       </c>
-      <c r="C84" s="43">
-        <v>12</v>
-      </c>
-      <c r="D84" s="47">
-        <v>85</v>
+      <c r="C84" s="76">
+        <v>0</v>
+      </c>
+      <c r="D84" s="81">
+        <v>0</v>
       </c>
       <c r="E84" s="12"/>
     </row>
-    <row r="85" spans="1:5">
-      <c r="A85" s="82">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A85" s="73">
         <v>42767.697916666664</v>
       </c>
-      <c r="B85" s="60" t="s">
+      <c r="B85" s="53" t="s">
         <v>143</v>
       </c>
-      <c r="C85" s="61">
-        <v>12</v>
-      </c>
-      <c r="D85" s="62">
-        <v>85</v>
+      <c r="C85" s="77">
+        <v>0</v>
+      </c>
+      <c r="D85" s="81">
+        <v>0</v>
       </c>
       <c r="E85" s="12"/>
     </row>
-    <row r="86" spans="1:5">
-      <c r="A86" s="81">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A86" s="72">
         <v>42767.708333333336</v>
       </c>
       <c r="B86" s="24" t="s">
         <v>145</v>
       </c>
-      <c r="C86" s="43">
-        <v>12</v>
-      </c>
-      <c r="D86" s="47">
-        <v>85</v>
+      <c r="C86" s="76">
+        <v>0</v>
+      </c>
+      <c r="D86" s="81">
+        <v>0</v>
       </c>
       <c r="E86" s="12"/>
     </row>
-    <row r="87" spans="1:5">
-      <c r="A87" s="81">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A87" s="72">
         <v>42767.71875</v>
       </c>
       <c r="B87" s="24" t="s">
         <v>147</v>
       </c>
-      <c r="C87" s="43">
-        <v>12</v>
-      </c>
-      <c r="D87" s="47">
-        <v>85</v>
+      <c r="C87" s="76">
+        <v>0</v>
+      </c>
+      <c r="D87" s="82">
+        <v>0</v>
       </c>
       <c r="E87" s="12"/>
     </row>
-    <row r="88" spans="1:5">
-      <c r="A88" s="81">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A88" s="72">
         <v>42767.729166666664</v>
       </c>
       <c r="B88" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="C88" s="43">
-        <v>12</v>
-      </c>
-      <c r="D88" s="47">
-        <v>85</v>
+      <c r="C88" s="76">
+        <v>0</v>
+      </c>
+      <c r="D88" s="81">
+        <v>0</v>
       </c>
       <c r="E88" s="12"/>
     </row>
-    <row r="89" spans="1:5">
-      <c r="A89" s="82">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A89" s="73">
         <v>42767.739583333336</v>
       </c>
-      <c r="B89" s="60" t="s">
+      <c r="B89" s="53" t="s">
         <v>151</v>
       </c>
-      <c r="C89" s="61">
-        <v>12</v>
-      </c>
-      <c r="D89" s="62">
-        <v>85</v>
+      <c r="C89" s="77">
+        <v>0</v>
+      </c>
+      <c r="D89" s="81">
+        <v>0</v>
       </c>
       <c r="E89" s="12"/>
     </row>
-    <row r="90" spans="1:5">
-      <c r="A90" s="81">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A90" s="72">
         <v>42767.75</v>
       </c>
       <c r="B90" s="24" t="s">
         <v>153</v>
       </c>
-      <c r="C90" s="43">
-        <v>12</v>
-      </c>
-      <c r="D90" s="47">
-        <v>85</v>
+      <c r="C90" s="76">
+        <v>0</v>
+      </c>
+      <c r="D90" s="81">
+        <v>0</v>
       </c>
       <c r="E90" s="12"/>
     </row>
-    <row r="91" spans="1:5">
-      <c r="A91" s="81">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A91" s="72">
         <v>42767.760416666664</v>
       </c>
       <c r="B91" s="24" t="s">
         <v>155</v>
       </c>
-      <c r="C91" s="43">
-        <v>12</v>
-      </c>
-      <c r="D91" s="47">
-        <v>85</v>
+      <c r="C91" s="76">
+        <v>0</v>
+      </c>
+      <c r="D91" s="81">
+        <v>0</v>
       </c>
       <c r="E91" s="12"/>
     </row>
-    <row r="92" spans="1:5">
-      <c r="A92" s="81">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A92" s="72">
         <v>42767.770833333336</v>
       </c>
       <c r="B92" s="24" t="s">
         <v>157</v>
       </c>
-      <c r="C92" s="43">
-        <v>12</v>
-      </c>
-      <c r="D92" s="47">
-        <v>85</v>
+      <c r="C92" s="76">
+        <v>0</v>
+      </c>
+      <c r="D92" s="82">
+        <v>0</v>
       </c>
       <c r="E92" s="12"/>
     </row>
-    <row r="93" spans="1:5">
-      <c r="A93" s="82">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A93" s="73">
         <v>42767.78125</v>
       </c>
-      <c r="B93" s="60" t="s">
+      <c r="B93" s="53" t="s">
         <v>159</v>
       </c>
-      <c r="C93" s="61">
-        <v>12</v>
-      </c>
-      <c r="D93" s="62">
-        <v>85</v>
+      <c r="C93" s="77">
+        <v>0</v>
+      </c>
+      <c r="D93" s="81">
+        <v>0</v>
       </c>
       <c r="E93" s="12"/>
     </row>
-    <row r="94" spans="1:5">
-      <c r="A94" s="81">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A94" s="72">
         <v>42767.791666666664</v>
       </c>
       <c r="B94" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="C94" s="43">
-        <v>0</v>
-      </c>
-      <c r="D94" s="47">
+      <c r="C94" s="76">
+        <v>0</v>
+      </c>
+      <c r="D94" s="81">
         <v>0</v>
       </c>
       <c r="E94" s="12"/>
     </row>
-    <row r="95" spans="1:5">
-      <c r="A95" s="81">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A95" s="72">
         <v>42767.802083333336</v>
       </c>
       <c r="B95" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="C95" s="43">
-        <v>0</v>
-      </c>
-      <c r="D95" s="47">
+      <c r="C95" s="76">
+        <v>0</v>
+      </c>
+      <c r="D95" s="81">
         <v>0</v>
       </c>
       <c r="E95" s="12"/>
     </row>
-    <row r="96" spans="1:5">
-      <c r="A96" s="81">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A96" s="72">
         <v>42767.8125</v>
       </c>
       <c r="B96" s="24" t="s">
         <v>165</v>
       </c>
-      <c r="C96" s="43">
-        <v>0</v>
-      </c>
-      <c r="D96" s="47">
+      <c r="C96" s="76">
+        <v>0</v>
+      </c>
+      <c r="D96" s="81">
         <v>0</v>
       </c>
       <c r="E96" s="12"/>
     </row>
-    <row r="97" spans="1:5">
-      <c r="A97" s="82">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A97" s="73">
         <v>42767.822916666664</v>
       </c>
-      <c r="B97" s="60" t="s">
+      <c r="B97" s="53" t="s">
         <v>167</v>
       </c>
-      <c r="C97" s="61">
-        <v>0</v>
-      </c>
-      <c r="D97" s="62">
+      <c r="C97" s="77">
+        <v>0</v>
+      </c>
+      <c r="D97" s="82">
         <v>0</v>
       </c>
       <c r="E97" s="12"/>
     </row>
-    <row r="98" spans="1:5">
-      <c r="A98" s="81">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A98" s="72">
         <v>42767.833333333336</v>
       </c>
       <c r="B98" s="24" t="s">
         <v>169</v>
       </c>
-      <c r="C98" s="43">
-        <v>0</v>
-      </c>
-      <c r="D98" s="47">
+      <c r="C98" s="76">
+        <v>0</v>
+      </c>
+      <c r="D98" s="81">
         <v>0</v>
       </c>
       <c r="E98" s="12"/>
     </row>
-    <row r="99" spans="1:5">
-      <c r="A99" s="81">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A99" s="72">
         <v>42767.84375</v>
       </c>
       <c r="B99" s="24" t="s">
         <v>171</v>
       </c>
-      <c r="C99" s="43">
-        <v>0</v>
-      </c>
-      <c r="D99" s="47">
+      <c r="C99" s="76">
+        <v>0</v>
+      </c>
+      <c r="D99" s="81">
         <v>0</v>
       </c>
       <c r="E99" s="12"/>
     </row>
-    <row r="100" spans="1:5">
-      <c r="A100" s="81">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A100" s="72">
         <v>42767.854166666664</v>
       </c>
       <c r="B100" s="24" t="s">
         <v>173</v>
       </c>
-      <c r="C100" s="43">
-        <v>0</v>
-      </c>
-      <c r="D100" s="47">
+      <c r="C100" s="76">
+        <v>0</v>
+      </c>
+      <c r="D100" s="81">
         <v>0</v>
       </c>
       <c r="E100" s="12"/>
     </row>
-    <row r="101" spans="1:5">
-      <c r="A101" s="82">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A101" s="73">
         <v>42767.864583333336</v>
       </c>
-      <c r="B101" s="60" t="s">
+      <c r="B101" s="53" t="s">
         <v>175</v>
       </c>
-      <c r="C101" s="61">
-        <v>0</v>
-      </c>
-      <c r="D101" s="62">
+      <c r="C101" s="77">
+        <v>0</v>
+      </c>
+      <c r="D101" s="81">
         <v>0</v>
       </c>
       <c r="E101" s="12"/>
     </row>
-    <row r="102" spans="1:5">
-      <c r="A102" s="81">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A102" s="72">
         <v>42767.875</v>
       </c>
       <c r="B102" s="24" t="s">
         <v>177</v>
       </c>
-      <c r="C102" s="43">
-        <v>0</v>
-      </c>
-      <c r="D102" s="47">
+      <c r="C102" s="76">
+        <v>0</v>
+      </c>
+      <c r="D102" s="81">
         <v>0</v>
       </c>
       <c r="E102" s="12"/>
     </row>
-    <row r="103" spans="1:5">
-      <c r="A103" s="81">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A103" s="72">
         <v>42767.885416666664</v>
       </c>
       <c r="B103" s="24" t="s">
         <v>179</v>
       </c>
-      <c r="C103" s="43">
-        <v>0</v>
-      </c>
-      <c r="D103" s="47">
+      <c r="C103" s="76">
+        <v>0</v>
+      </c>
+      <c r="D103" s="81">
         <v>0</v>
       </c>
       <c r="E103" s="12"/>
     </row>
-    <row r="104" spans="1:5">
-      <c r="A104" s="81">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A104" s="72">
         <v>42767.895833333336</v>
       </c>
       <c r="B104" s="24" t="s">
         <v>181</v>
       </c>
-      <c r="C104" s="43">
-        <v>0</v>
-      </c>
-      <c r="D104" s="47">
+      <c r="C104" s="76">
+        <v>0</v>
+      </c>
+      <c r="D104" s="81">
         <v>0</v>
       </c>
       <c r="E104" s="12"/>
     </row>
-    <row r="105" spans="1:5">
-      <c r="A105" s="82">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A105" s="73">
         <v>42767.90625</v>
       </c>
-      <c r="B105" s="60" t="s">
+      <c r="B105" s="53" t="s">
         <v>183</v>
       </c>
-      <c r="C105" s="61">
-        <v>0</v>
-      </c>
-      <c r="D105" s="62">
+      <c r="C105" s="77">
+        <v>0</v>
+      </c>
+      <c r="D105" s="82">
         <v>0</v>
       </c>
       <c r="E105" s="12"/>
     </row>
-    <row r="106" spans="1:5">
-      <c r="A106" s="81">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A106" s="72">
         <v>42767.916666666664</v>
       </c>
       <c r="B106" s="24" t="s">
         <v>185</v>
       </c>
-      <c r="C106" s="43">
-        <v>0</v>
-      </c>
-      <c r="D106" s="47">
+      <c r="C106" s="76">
+        <v>0</v>
+      </c>
+      <c r="D106" s="81">
         <v>0</v>
       </c>
       <c r="E106" s="12"/>
     </row>
-    <row r="107" spans="1:5">
-      <c r="A107" s="81">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A107" s="72">
         <v>42767.927083333336</v>
       </c>
       <c r="B107" s="24" t="s">
         <v>187</v>
       </c>
-      <c r="C107" s="43">
-        <v>0</v>
-      </c>
-      <c r="D107" s="47">
+      <c r="C107" s="76">
+        <v>0</v>
+      </c>
+      <c r="D107" s="81">
         <v>0</v>
       </c>
       <c r="E107" s="12"/>
     </row>
-    <row r="108" spans="1:5">
-      <c r="A108" s="81">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A108" s="72">
         <v>42767.9375</v>
       </c>
       <c r="B108" s="24" t="s">
         <v>189</v>
       </c>
-      <c r="C108" s="43">
-        <v>0</v>
-      </c>
-      <c r="D108" s="47">
+      <c r="C108" s="76">
+        <v>0</v>
+      </c>
+      <c r="D108" s="81">
         <v>0</v>
       </c>
       <c r="E108" s="12"/>
     </row>
-    <row r="109" spans="1:5">
-      <c r="A109" s="82">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A109" s="73">
         <v>42767.947916666664</v>
       </c>
-      <c r="B109" s="60" t="s">
+      <c r="B109" s="53" t="s">
         <v>191</v>
       </c>
-      <c r="C109" s="61">
-        <v>0</v>
-      </c>
-      <c r="D109" s="62">
+      <c r="C109" s="77">
+        <v>0</v>
+      </c>
+      <c r="D109" s="82">
         <v>0</v>
       </c>
       <c r="E109" s="12"/>
     </row>
-    <row r="110" spans="1:5">
-      <c r="A110" s="81">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A110" s="72">
         <v>42767.958333333336</v>
       </c>
       <c r="B110" s="24" t="s">
         <v>193</v>
       </c>
-      <c r="C110" s="43">
-        <v>0</v>
-      </c>
-      <c r="D110" s="47">
+      <c r="C110" s="76">
+        <v>0</v>
+      </c>
+      <c r="D110" s="81">
         <v>0</v>
       </c>
       <c r="E110" s="12"/>
     </row>
-    <row r="111" spans="1:5">
-      <c r="A111" s="81">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A111" s="72">
         <v>42767.96875</v>
       </c>
       <c r="B111" s="24" t="s">
         <v>195</v>
       </c>
-      <c r="C111" s="43">
-        <v>0</v>
-      </c>
-      <c r="D111" s="47">
+      <c r="C111" s="76">
+        <v>0</v>
+      </c>
+      <c r="D111" s="81">
         <v>0</v>
       </c>
       <c r="E111" s="12"/>
     </row>
-    <row r="112" spans="1:5">
-      <c r="A112" s="81">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A112" s="72">
         <v>42767.979166666664</v>
       </c>
       <c r="B112" s="24" t="s">
         <v>197</v>
       </c>
-      <c r="C112" s="43">
-        <v>0</v>
-      </c>
-      <c r="D112" s="47">
+      <c r="C112" s="76">
+        <v>0</v>
+      </c>
+      <c r="D112" s="81">
         <v>0</v>
       </c>
       <c r="E112" s="12"/>
     </row>
-    <row r="113" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A113" s="83">
+    <row r="113" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="74">
         <v>42767.989583333336</v>
       </c>
       <c r="B113" s="33" t="s">
         <v>199</v>
       </c>
-      <c r="C113" s="44">
-        <v>0</v>
-      </c>
-      <c r="D113" s="48">
+      <c r="C113" s="78">
+        <v>0</v>
+      </c>
+      <c r="D113" s="83">
         <v>0</v>
       </c>
       <c r="E113" s="12"/>
     </row>
-    <row r="114" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A114" s="58"/>
+    <row r="114" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="51"/>
       <c r="B114" s="27" t="s">
         <v>221</v>
       </c>
-      <c r="C114" s="45">
-        <v>36</v>
-      </c>
-      <c r="D114" s="45"/>
+      <c r="C114" s="79">
+        <v>0</v>
+      </c>
+      <c r="D114" s="84"/>
       <c r="E114" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C114"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="13.5" thickBot="1">
-      <c r="A1" s="49" t="s">
+    <row r="1" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="42" t="s">
         <v>222</v>
       </c>
-      <c r="B1" s="64" t="s">
+      <c r="B1" s="55" t="s">
         <v>207</v>
       </c>
-      <c r="C1" s="63"/>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="C1" s="54"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
         <v>206</v>
       </c>
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="65" t="s">
         <v>208</v>
       </c>
       <c r="C2" s="13"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="17"/>
-      <c r="B3" s="65" t="s">
+      <c r="B3" s="56" t="s">
         <v>209</v>
       </c>
       <c r="C3" s="13"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="17"/>
-      <c r="B4" s="66" t="s">
+      <c r="B4" s="57" t="s">
         <v>210</v>
       </c>
       <c r="C4" s="14"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="17"/>
-      <c r="B5" s="66" t="s">
+      <c r="B5" s="57" t="s">
         <v>211</v>
       </c>
       <c r="C5" s="14"/>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="17"/>
-      <c r="B6" s="67"/>
+      <c r="B6" s="58"/>
       <c r="C6" s="14"/>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="17"/>
-      <c r="B7" s="66" t="s">
+      <c r="B7" s="57" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="14"/>
     </row>
-    <row r="8" spans="1:3" ht="13.5" thickBot="1">
+    <row r="8" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="29"/>
-      <c r="B8" s="75" t="s">
+      <c r="B8" s="66" t="s">
         <v>212</v>
       </c>
       <c r="C8" s="13"/>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="50" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="43" t="s">
         <v>213</v>
       </c>
-      <c r="B9" s="68" t="s">
+      <c r="B9" s="59" t="s">
         <v>215</v>
       </c>
       <c r="C9" s="12"/>
     </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="51"/>
-      <c r="B10" s="68" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="44"/>
+      <c r="B10" s="59" t="s">
         <v>217</v>
       </c>
       <c r="C10" s="12"/>
     </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="51"/>
-      <c r="B11" s="68" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="44"/>
+      <c r="B11" s="59" t="s">
         <v>216</v>
       </c>
       <c r="C11" s="12"/>
     </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="51"/>
-      <c r="B12" s="68" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="44"/>
+      <c r="B12" s="59" t="s">
         <v>217</v>
       </c>
       <c r="C12" s="12"/>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="51"/>
-      <c r="B13" s="69"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="44"/>
+      <c r="B13" s="60"/>
       <c r="C13" s="12"/>
     </row>
-    <row r="14" spans="1:3" ht="13.5" thickBot="1">
-      <c r="A14" s="51"/>
-      <c r="B14" s="69"/>
+    <row r="14" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="44"/>
+      <c r="B14" s="60"/>
       <c r="C14" s="12"/>
     </row>
-    <row r="15" spans="1:3" ht="13.5" thickBot="1">
-      <c r="A15" s="52" t="s">
+    <row r="15" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="45" t="s">
         <v>214</v>
       </c>
-      <c r="B15" s="76" t="s">
+      <c r="B15" s="67" t="s">
         <v>218</v>
       </c>
       <c r="C15" s="15"/>
     </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="53"/>
-      <c r="B16" s="70"/>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="46"/>
+      <c r="B16" s="61"/>
       <c r="C16" s="15"/>
     </row>
-    <row r="17" spans="1:3" ht="13.5" thickBot="1">
-      <c r="A17" s="54" t="s">
+    <row r="17" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="47" t="s">
         <v>219</v>
       </c>
-      <c r="B17" s="71" t="s">
+      <c r="B17" s="62" t="s">
         <v>220</v>
       </c>
       <c r="C17" s="15"/>
     </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="55" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="77" t="s">
+      <c r="B18" s="68" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="12"/>
     </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="56" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="72" t="s">
+      <c r="B19" s="63" t="s">
         <v>11</v>
       </c>
       <c r="C19" s="12"/>
     </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="56" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="72" t="s">
+      <c r="B20" s="63" t="s">
         <v>13</v>
       </c>
       <c r="C20" s="12"/>
     </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="59" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="79" t="s">
+      <c r="B21" s="70" t="s">
         <v>15</v>
       </c>
       <c r="C21" s="12"/>
     </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="56" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="72" t="s">
+      <c r="B22" s="63" t="s">
         <v>17</v>
       </c>
       <c r="C22" s="12"/>
     </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="56" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="72" t="s">
+      <c r="B23" s="63" t="s">
         <v>19</v>
       </c>
       <c r="C23" s="12"/>
     </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="56" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="72" t="s">
+      <c r="B24" s="63" t="s">
         <v>21</v>
       </c>
       <c r="C24" s="12"/>
     </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="59" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="79" t="s">
+      <c r="B25" s="70" t="s">
         <v>23</v>
       </c>
       <c r="C25" s="12"/>
     </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="56" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="72" t="s">
+      <c r="B26" s="63" t="s">
         <v>25</v>
       </c>
       <c r="C26" s="12"/>
     </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="56" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="72" t="s">
+      <c r="B27" s="63" t="s">
         <v>27</v>
       </c>
       <c r="C27" s="12"/>
     </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="56" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="72" t="s">
+      <c r="B28" s="63" t="s">
         <v>29</v>
       </c>
       <c r="C28" s="12"/>
     </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="59" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="B29" s="79" t="s">
+      <c r="B29" s="70" t="s">
         <v>31</v>
       </c>
       <c r="C29" s="12"/>
     </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="56" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="72" t="s">
+      <c r="B30" s="63" t="s">
         <v>33</v>
       </c>
       <c r="C30" s="12"/>
     </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="56" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="72" t="s">
+      <c r="B31" s="63" t="s">
         <v>35</v>
       </c>
       <c r="C31" s="12"/>
     </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="56" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="72" t="s">
+      <c r="B32" s="63" t="s">
         <v>37</v>
       </c>
       <c r="C32" s="12"/>
     </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="59" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="79" t="s">
+      <c r="B33" s="70" t="s">
         <v>39</v>
       </c>
       <c r="C33" s="12"/>
     </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="56" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="B34" s="72" t="s">
+      <c r="B34" s="63" t="s">
         <v>41</v>
       </c>
       <c r="C34" s="12"/>
     </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="56" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="B35" s="72" t="s">
+      <c r="B35" s="63" t="s">
         <v>43</v>
       </c>
       <c r="C35" s="12"/>
     </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="56" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="B36" s="72" t="s">
+      <c r="B36" s="63" t="s">
         <v>45</v>
       </c>
       <c r="C36" s="12"/>
     </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="59" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="B37" s="79" t="s">
+      <c r="B37" s="70" t="s">
         <v>47</v>
       </c>
       <c r="C37" s="12"/>
     </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="56" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="B38" s="72" t="s">
+      <c r="B38" s="63" t="s">
         <v>49</v>
       </c>
       <c r="C38" s="12"/>
     </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="56" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="B39" s="72" t="s">
+      <c r="B39" s="63" t="s">
         <v>51</v>
       </c>
       <c r="C39" s="12"/>
     </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="56" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="B40" s="72" t="s">
+      <c r="B40" s="63" t="s">
         <v>53</v>
       </c>
       <c r="C40" s="12"/>
     </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="59" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="B41" s="79" t="s">
+      <c r="B41" s="70" t="s">
         <v>55</v>
       </c>
       <c r="C41" s="12"/>
     </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="56" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="B42" s="72" t="s">
+      <c r="B42" s="63" t="s">
         <v>57</v>
       </c>
       <c r="C42" s="12"/>
     </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="56" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="B43" s="72" t="s">
+      <c r="B43" s="63" t="s">
         <v>59</v>
       </c>
       <c r="C43" s="12"/>
     </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="56" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="B44" s="72" t="s">
+      <c r="B44" s="63" t="s">
         <v>61</v>
       </c>
       <c r="C44" s="12"/>
     </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="59" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="52" t="s">
         <v>62</v>
       </c>
-      <c r="B45" s="79" t="s">
+      <c r="B45" s="70" t="s">
         <v>63</v>
       </c>
       <c r="C45" s="12"/>
     </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="56" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="B46" s="72" t="s">
+      <c r="B46" s="63" t="s">
         <v>65</v>
       </c>
       <c r="C46" s="12"/>
     </row>
-    <row r="47" spans="1:3">
-      <c r="A47" s="56" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="B47" s="72" t="s">
+      <c r="B47" s="63" t="s">
         <v>67</v>
       </c>
       <c r="C47" s="12"/>
     </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="56" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="B48" s="72" t="s">
+      <c r="B48" s="63" t="s">
         <v>69</v>
       </c>
       <c r="C48" s="12"/>
     </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="59" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="52" t="s">
         <v>70</v>
       </c>
-      <c r="B49" s="79" t="s">
+      <c r="B49" s="70" t="s">
         <v>71</v>
       </c>
       <c r="C49" s="12"/>
     </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="56" t="s">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="B50" s="72" t="s">
+      <c r="B50" s="63" t="s">
         <v>73</v>
       </c>
       <c r="C50" s="12"/>
     </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="56" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="B51" s="72" t="s">
+      <c r="B51" s="63" t="s">
         <v>75</v>
       </c>
       <c r="C51" s="12"/>
     </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="56" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="B52" s="72" t="s">
+      <c r="B52" s="63" t="s">
         <v>77</v>
       </c>
       <c r="C52" s="12"/>
     </row>
-    <row r="53" spans="1:3">
-      <c r="A53" s="59" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="52" t="s">
         <v>78</v>
       </c>
-      <c r="B53" s="79" t="s">
+      <c r="B53" s="70" t="s">
         <v>79</v>
       </c>
       <c r="C53" s="12"/>
     </row>
-    <row r="54" spans="1:3">
-      <c r="A54" s="56" t="s">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="B54" s="72" t="s">
+      <c r="B54" s="63" t="s">
         <v>81</v>
       </c>
       <c r="C54" s="12"/>
     </row>
-    <row r="55" spans="1:3">
-      <c r="A55" s="56" t="s">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="49" t="s">
         <v>82</v>
       </c>
-      <c r="B55" s="72" t="s">
+      <c r="B55" s="63" t="s">
         <v>83</v>
       </c>
       <c r="C55" s="12"/>
     </row>
-    <row r="56" spans="1:3">
-      <c r="A56" s="56" t="s">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="49" t="s">
         <v>84</v>
       </c>
-      <c r="B56" s="72" t="s">
+      <c r="B56" s="63" t="s">
         <v>85</v>
       </c>
       <c r="C56" s="12"/>
     </row>
-    <row r="57" spans="1:3">
-      <c r="A57" s="59" t="s">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="52" t="s">
         <v>86</v>
       </c>
-      <c r="B57" s="79" t="s">
+      <c r="B57" s="70" t="s">
         <v>87</v>
       </c>
       <c r="C57" s="12"/>
     </row>
-    <row r="58" spans="1:3">
-      <c r="A58" s="56" t="s">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="B58" s="72" t="s">
+      <c r="B58" s="63" t="s">
         <v>89</v>
       </c>
       <c r="C58" s="12"/>
     </row>
-    <row r="59" spans="1:3">
-      <c r="A59" s="56" t="s">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="49" t="s">
         <v>90</v>
       </c>
-      <c r="B59" s="72" t="s">
+      <c r="B59" s="63" t="s">
         <v>91</v>
       </c>
       <c r="C59" s="12"/>
     </row>
-    <row r="60" spans="1:3">
-      <c r="A60" s="56" t="s">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="49" t="s">
         <v>92</v>
       </c>
-      <c r="B60" s="72" t="s">
+      <c r="B60" s="63" t="s">
         <v>93</v>
       </c>
       <c r="C60" s="12"/>
     </row>
-    <row r="61" spans="1:3">
-      <c r="A61" s="59" t="s">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="52" t="s">
         <v>94</v>
       </c>
-      <c r="B61" s="79" t="s">
+      <c r="B61" s="70" t="s">
         <v>95</v>
       </c>
       <c r="C61" s="12"/>
     </row>
-    <row r="62" spans="1:3">
-      <c r="A62" s="56" t="s">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="B62" s="72" t="s">
+      <c r="B62" s="63" t="s">
         <v>97</v>
       </c>
       <c r="C62" s="12"/>
     </row>
-    <row r="63" spans="1:3">
-      <c r="A63" s="56" t="s">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="B63" s="72" t="s">
+      <c r="B63" s="63" t="s">
         <v>99</v>
       </c>
       <c r="C63" s="12"/>
     </row>
-    <row r="64" spans="1:3">
-      <c r="A64" s="56" t="s">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="49" t="s">
         <v>100</v>
       </c>
-      <c r="B64" s="72" t="s">
+      <c r="B64" s="63" t="s">
         <v>101</v>
       </c>
       <c r="C64" s="12"/>
     </row>
-    <row r="65" spans="1:3">
-      <c r="A65" s="59" t="s">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="52" t="s">
         <v>102</v>
       </c>
-      <c r="B65" s="79" t="s">
+      <c r="B65" s="70" t="s">
         <v>103</v>
       </c>
       <c r="C65" s="12"/>
     </row>
-    <row r="66" spans="1:3">
-      <c r="A66" s="56" t="s">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="49" t="s">
         <v>104</v>
       </c>
-      <c r="B66" s="72" t="s">
+      <c r="B66" s="63" t="s">
         <v>105</v>
       </c>
       <c r="C66" s="12"/>
     </row>
-    <row r="67" spans="1:3">
-      <c r="A67" s="56" t="s">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="49" t="s">
         <v>106</v>
       </c>
-      <c r="B67" s="72" t="s">
+      <c r="B67" s="63" t="s">
         <v>107</v>
       </c>
       <c r="C67" s="12"/>
     </row>
-    <row r="68" spans="1:3">
-      <c r="A68" s="56" t="s">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="49" t="s">
         <v>108</v>
       </c>
-      <c r="B68" s="72" t="s">
+      <c r="B68" s="63" t="s">
         <v>109</v>
       </c>
       <c r="C68" s="12"/>
     </row>
-    <row r="69" spans="1:3">
-      <c r="A69" s="59" t="s">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="52" t="s">
         <v>110</v>
       </c>
-      <c r="B69" s="79" t="s">
+      <c r="B69" s="70" t="s">
         <v>111</v>
       </c>
       <c r="C69" s="12"/>
     </row>
-    <row r="70" spans="1:3">
-      <c r="A70" s="56" t="s">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="49" t="s">
         <v>112</v>
       </c>
-      <c r="B70" s="72" t="s">
+      <c r="B70" s="63" t="s">
         <v>113</v>
       </c>
       <c r="C70" s="12"/>
     </row>
-    <row r="71" spans="1:3">
-      <c r="A71" s="56" t="s">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="49" t="s">
         <v>114</v>
       </c>
-      <c r="B71" s="72" t="s">
+      <c r="B71" s="63" t="s">
         <v>115</v>
       </c>
       <c r="C71" s="12"/>
     </row>
-    <row r="72" spans="1:3">
-      <c r="A72" s="56" t="s">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="49" t="s">
         <v>116</v>
       </c>
-      <c r="B72" s="72" t="s">
+      <c r="B72" s="63" t="s">
         <v>117</v>
       </c>
       <c r="C72" s="12"/>
     </row>
-    <row r="73" spans="1:3">
-      <c r="A73" s="59" t="s">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="B73" s="79" t="s">
+      <c r="B73" s="70" t="s">
         <v>119</v>
       </c>
       <c r="C73" s="12"/>
     </row>
-    <row r="74" spans="1:3">
-      <c r="A74" s="56" t="s">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" s="49" t="s">
         <v>120</v>
       </c>
-      <c r="B74" s="72" t="s">
+      <c r="B74" s="63" t="s">
         <v>121</v>
       </c>
       <c r="C74" s="12"/>
     </row>
-    <row r="75" spans="1:3">
-      <c r="A75" s="56" t="s">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="49" t="s">
         <v>122</v>
       </c>
-      <c r="B75" s="72" t="s">
+      <c r="B75" s="63" t="s">
         <v>123</v>
       </c>
       <c r="C75" s="12"/>
     </row>
-    <row r="76" spans="1:3">
-      <c r="A76" s="56" t="s">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" s="49" t="s">
         <v>124</v>
       </c>
-      <c r="B76" s="72" t="s">
+      <c r="B76" s="63" t="s">
         <v>125</v>
       </c>
       <c r="C76" s="12"/>
     </row>
-    <row r="77" spans="1:3">
-      <c r="A77" s="59" t="s">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" s="52" t="s">
         <v>126</v>
       </c>
-      <c r="B77" s="79" t="s">
+      <c r="B77" s="70" t="s">
         <v>127</v>
       </c>
       <c r="C77" s="12"/>
     </row>
-    <row r="78" spans="1:3">
-      <c r="A78" s="56" t="s">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="49" t="s">
         <v>128</v>
       </c>
-      <c r="B78" s="72" t="s">
+      <c r="B78" s="63" t="s">
         <v>129</v>
       </c>
       <c r="C78" s="12"/>
     </row>
-    <row r="79" spans="1:3">
-      <c r="A79" s="56" t="s">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="B79" s="72" t="s">
+      <c r="B79" s="63" t="s">
         <v>131</v>
       </c>
       <c r="C79" s="12"/>
     </row>
-    <row r="80" spans="1:3">
-      <c r="A80" s="56" t="s">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" s="49" t="s">
         <v>132</v>
       </c>
-      <c r="B80" s="72" t="s">
+      <c r="B80" s="63" t="s">
         <v>133</v>
       </c>
       <c r="C80" s="12"/>
     </row>
-    <row r="81" spans="1:3">
-      <c r="A81" s="59" t="s">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" s="52" t="s">
         <v>134</v>
       </c>
-      <c r="B81" s="79" t="s">
+      <c r="B81" s="70" t="s">
         <v>135</v>
       </c>
       <c r="C81" s="12"/>
     </row>
-    <row r="82" spans="1:3">
-      <c r="A82" s="56" t="s">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" s="49" t="s">
         <v>136</v>
       </c>
-      <c r="B82" s="72" t="s">
+      <c r="B82" s="63" t="s">
         <v>137</v>
       </c>
       <c r="C82" s="12"/>
     </row>
-    <row r="83" spans="1:3">
-      <c r="A83" s="56" t="s">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" s="49" t="s">
         <v>138</v>
       </c>
-      <c r="B83" s="72" t="s">
+      <c r="B83" s="63" t="s">
         <v>139</v>
       </c>
       <c r="C83" s="12"/>
     </row>
-    <row r="84" spans="1:3">
-      <c r="A84" s="56" t="s">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" s="49" t="s">
         <v>140</v>
       </c>
-      <c r="B84" s="72" t="s">
+      <c r="B84" s="63" t="s">
         <v>141</v>
       </c>
       <c r="C84" s="12"/>
     </row>
-    <row r="85" spans="1:3">
-      <c r="A85" s="59" t="s">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" s="52" t="s">
         <v>142</v>
       </c>
-      <c r="B85" s="79" t="s">
+      <c r="B85" s="70" t="s">
         <v>143</v>
       </c>
       <c r="C85" s="12"/>
     </row>
-    <row r="86" spans="1:3">
-      <c r="A86" s="56" t="s">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" s="49" t="s">
         <v>144</v>
       </c>
-      <c r="B86" s="72" t="s">
+      <c r="B86" s="63" t="s">
         <v>145</v>
       </c>
       <c r="C86" s="12"/>
     </row>
-    <row r="87" spans="1:3">
-      <c r="A87" s="56" t="s">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" s="49" t="s">
         <v>146</v>
       </c>
-      <c r="B87" s="72" t="s">
+      <c r="B87" s="63" t="s">
         <v>147</v>
       </c>
       <c r="C87" s="12"/>
     </row>
-    <row r="88" spans="1:3">
-      <c r="A88" s="56" t="s">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" s="49" t="s">
         <v>148</v>
       </c>
-      <c r="B88" s="72" t="s">
+      <c r="B88" s="63" t="s">
         <v>149</v>
       </c>
       <c r="C88" s="12"/>
     </row>
-    <row r="89" spans="1:3">
-      <c r="A89" s="59" t="s">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" s="52" t="s">
         <v>150</v>
       </c>
-      <c r="B89" s="79" t="s">
+      <c r="B89" s="70" t="s">
         <v>151</v>
       </c>
       <c r="C89" s="12"/>
     </row>
-    <row r="90" spans="1:3">
-      <c r="A90" s="56" t="s">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" s="49" t="s">
         <v>152</v>
       </c>
-      <c r="B90" s="72" t="s">
+      <c r="B90" s="63" t="s">
         <v>153</v>
       </c>
       <c r="C90" s="12"/>
     </row>
-    <row r="91" spans="1:3">
-      <c r="A91" s="56" t="s">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" s="49" t="s">
         <v>154</v>
       </c>
-      <c r="B91" s="72" t="s">
+      <c r="B91" s="63" t="s">
         <v>155</v>
       </c>
       <c r="C91" s="12"/>
     </row>
-    <row r="92" spans="1:3">
-      <c r="A92" s="56" t="s">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" s="49" t="s">
         <v>156</v>
       </c>
-      <c r="B92" s="72" t="s">
+      <c r="B92" s="63" t="s">
         <v>157</v>
       </c>
       <c r="C92" s="12"/>
     </row>
-    <row r="93" spans="1:3">
-      <c r="A93" s="59" t="s">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" s="52" t="s">
         <v>158</v>
       </c>
-      <c r="B93" s="79" t="s">
+      <c r="B93" s="70" t="s">
         <v>159</v>
       </c>
       <c r="C93" s="12"/>
     </row>
-    <row r="94" spans="1:3">
-      <c r="A94" s="56" t="s">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" s="49" t="s">
         <v>160</v>
       </c>
-      <c r="B94" s="72" t="s">
+      <c r="B94" s="63" t="s">
         <v>161</v>
       </c>
       <c r="C94" s="12"/>
     </row>
-    <row r="95" spans="1:3">
-      <c r="A95" s="56" t="s">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" s="49" t="s">
         <v>162</v>
       </c>
-      <c r="B95" s="72" t="s">
+      <c r="B95" s="63" t="s">
         <v>163</v>
       </c>
       <c r="C95" s="12"/>
     </row>
-    <row r="96" spans="1:3">
-      <c r="A96" s="56" t="s">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" s="49" t="s">
         <v>164</v>
       </c>
-      <c r="B96" s="72" t="s">
+      <c r="B96" s="63" t="s">
         <v>165</v>
       </c>
       <c r="C96" s="12"/>
     </row>
-    <row r="97" spans="1:3">
-      <c r="A97" s="59" t="s">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" s="52" t="s">
         <v>166</v>
       </c>
-      <c r="B97" s="79" t="s">
+      <c r="B97" s="70" t="s">
         <v>167</v>
       </c>
       <c r="C97" s="12"/>
     </row>
-    <row r="98" spans="1:3">
-      <c r="A98" s="56" t="s">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" s="49" t="s">
         <v>168</v>
       </c>
-      <c r="B98" s="72" t="s">
+      <c r="B98" s="63" t="s">
         <v>169</v>
       </c>
       <c r="C98" s="12"/>
     </row>
-    <row r="99" spans="1:3">
-      <c r="A99" s="56" t="s">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" s="49" t="s">
         <v>170</v>
       </c>
-      <c r="B99" s="72" t="s">
+      <c r="B99" s="63" t="s">
         <v>171</v>
       </c>
       <c r="C99" s="12"/>
     </row>
-    <row r="100" spans="1:3">
-      <c r="A100" s="56" t="s">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100" s="49" t="s">
         <v>172</v>
       </c>
-      <c r="B100" s="72" t="s">
+      <c r="B100" s="63" t="s">
         <v>173</v>
       </c>
       <c r="C100" s="12"/>
     </row>
-    <row r="101" spans="1:3">
-      <c r="A101" s="59" t="s">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101" s="52" t="s">
         <v>174</v>
       </c>
-      <c r="B101" s="79" t="s">
+      <c r="B101" s="70" t="s">
         <v>175</v>
       </c>
       <c r="C101" s="12"/>
     </row>
-    <row r="102" spans="1:3">
-      <c r="A102" s="56" t="s">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102" s="49" t="s">
         <v>176</v>
       </c>
-      <c r="B102" s="72" t="s">
+      <c r="B102" s="63" t="s">
         <v>177</v>
       </c>
       <c r="C102" s="12"/>
     </row>
-    <row r="103" spans="1:3">
-      <c r="A103" s="56" t="s">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A103" s="49" t="s">
         <v>178</v>
       </c>
-      <c r="B103" s="72" t="s">
+      <c r="B103" s="63" t="s">
         <v>179</v>
       </c>
       <c r="C103" s="12"/>
     </row>
-    <row r="104" spans="1:3">
-      <c r="A104" s="56" t="s">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104" s="49" t="s">
         <v>180</v>
       </c>
-      <c r="B104" s="72" t="s">
+      <c r="B104" s="63" t="s">
         <v>181</v>
       </c>
       <c r="C104" s="12"/>
     </row>
-    <row r="105" spans="1:3">
-      <c r="A105" s="59" t="s">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A105" s="52" t="s">
         <v>182</v>
       </c>
-      <c r="B105" s="79" t="s">
+      <c r="B105" s="70" t="s">
         <v>183</v>
       </c>
       <c r="C105" s="12"/>
     </row>
-    <row r="106" spans="1:3">
-      <c r="A106" s="56" t="s">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A106" s="49" t="s">
         <v>184</v>
       </c>
-      <c r="B106" s="72" t="s">
+      <c r="B106" s="63" t="s">
         <v>185</v>
       </c>
       <c r="C106" s="12"/>
     </row>
-    <row r="107" spans="1:3">
-      <c r="A107" s="56" t="s">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A107" s="49" t="s">
         <v>186</v>
       </c>
-      <c r="B107" s="72" t="s">
+      <c r="B107" s="63" t="s">
         <v>187</v>
       </c>
       <c r="C107" s="12"/>
     </row>
-    <row r="108" spans="1:3">
-      <c r="A108" s="56" t="s">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A108" s="49" t="s">
         <v>188</v>
       </c>
-      <c r="B108" s="72" t="s">
+      <c r="B108" s="63" t="s">
         <v>189</v>
       </c>
       <c r="C108" s="12"/>
     </row>
-    <row r="109" spans="1:3">
-      <c r="A109" s="59" t="s">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A109" s="52" t="s">
         <v>190</v>
       </c>
-      <c r="B109" s="79" t="s">
+      <c r="B109" s="70" t="s">
         <v>191</v>
       </c>
       <c r="C109" s="12"/>
     </row>
-    <row r="110" spans="1:3">
-      <c r="A110" s="56" t="s">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A110" s="49" t="s">
         <v>192</v>
       </c>
-      <c r="B110" s="72" t="s">
+      <c r="B110" s="63" t="s">
         <v>193</v>
       </c>
       <c r="C110" s="12"/>
     </row>
-    <row r="111" spans="1:3">
-      <c r="A111" s="56" t="s">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A111" s="49" t="s">
         <v>194</v>
       </c>
-      <c r="B111" s="72" t="s">
+      <c r="B111" s="63" t="s">
         <v>195</v>
       </c>
       <c r="C111" s="12"/>
     </row>
-    <row r="112" spans="1:3">
-      <c r="A112" s="56" t="s">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A112" s="49" t="s">
         <v>196</v>
       </c>
-      <c r="B112" s="72" t="s">
+      <c r="B112" s="63" t="s">
         <v>197</v>
       </c>
       <c r="C112" s="12"/>
     </row>
-    <row r="113" spans="1:3" ht="13.5" thickBot="1">
-      <c r="A113" s="57" t="s">
+    <row r="113" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="50" t="s">
         <v>198</v>
       </c>
-      <c r="B113" s="78" t="s">
+      <c r="B113" s="69" t="s">
         <v>199</v>
       </c>
       <c r="C113" s="12"/>
     </row>
-    <row r="114" spans="1:3" ht="13.5" thickBot="1">
-      <c r="A114" s="58"/>
-      <c r="B114" s="73" t="s">
+    <row r="114" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="51"/>
+      <c r="B114" s="64" t="s">
         <v>221</v>
       </c>
       <c r="C114" s="15"/>

</xml_diff>

<commit_message>
Added Some Formatting to the Output KISS file
</commit_message>
<xml_diff>
--- a/HkwgConverter/Sample/Template_Kiss_Input.xlsx
+++ b/HkwgConverter/Sample/Template_Kiss_Input.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="223">
   <si>
     <t>Info</t>
   </si>
@@ -691,11 +691,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
     <numFmt numFmtId="165" formatCode="#,##0.000\ &quot;MWh&quot;"/>
     <numFmt numFmtId="166" formatCode="0.000;[Red]0.000"/>
-    <numFmt numFmtId="167" formatCode="0.00;[Red]0.00"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -750,7 +749,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -775,14 +774,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="42"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="23">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -1002,31 +995,9 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -1048,7 +1019,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1109,16 +1080,10 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1131,12 +1096,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1185,10 +1144,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="0" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1233,49 +1189,7 @@
     <xf numFmtId="20" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="0" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1639,10 +1553,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E114"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1653,31 +1567,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="38" t="s">
         <v>205</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="25" t="s">
         <v>207</v>
       </c>
-      <c r="C1" s="34">
+      <c r="C1" s="30">
         <v>42767</v>
       </c>
-      <c r="D1" s="34">
+      <c r="D1" s="30">
         <v>42767</v>
       </c>
       <c r="E1" s="12"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="24" t="s">
         <v>206</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="26" t="s">
         <v>208</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="31" t="s">
         <v>201</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="31" t="s">
         <v>201</v>
       </c>
       <c r="E2" s="13"/>
@@ -1687,10 +1601,10 @@
       <c r="B3" s="16" t="s">
         <v>209</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="32" t="s">
         <v>201</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="32" t="s">
         <v>201</v>
       </c>
       <c r="E3" s="13"/>
@@ -1700,10 +1614,10 @@
       <c r="B4" s="18" t="s">
         <v>210</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="33" t="s">
         <v>202</v>
       </c>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="33" t="s">
         <v>202</v>
       </c>
       <c r="E4" s="14"/>
@@ -1713,10 +1627,10 @@
       <c r="B5" s="18" t="s">
         <v>211</v>
       </c>
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="37" t="s">
+      <c r="D5" s="33" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="14"/>
@@ -1724,8 +1638,8 @@
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="17"/>
       <c r="B6" s="19"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
       <c r="E6" s="14"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1733,1572 +1647,121 @@
       <c r="B7" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="37" t="s">
+      <c r="C7" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="37" t="s">
+      <c r="D7" s="33" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="14"/>
     </row>
     <row r="8" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="29"/>
-      <c r="B8" s="30" t="s">
+      <c r="A8" s="27"/>
+      <c r="B8" s="28" t="s">
         <v>212</v>
       </c>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
       <c r="E8" s="13"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="39" t="s">
         <v>213</v>
       </c>
       <c r="B9" s="20" t="s">
         <v>215</v>
       </c>
-      <c r="C9" s="39" t="s">
+      <c r="C9" s="35" t="s">
         <v>203</v>
       </c>
-      <c r="D9" s="39" t="s">
+      <c r="D9" s="35" t="s">
         <v>203</v>
       </c>
       <c r="E9" s="12"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="44"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="20" t="s">
         <v>217</v>
       </c>
-      <c r="C10" s="39" t="s">
+      <c r="C10" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="39" t="s">
+      <c r="D10" s="35" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="12"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="44"/>
+      <c r="A11" s="40"/>
       <c r="B11" s="20" t="s">
         <v>216</v>
       </c>
-      <c r="C11" s="39" t="s">
+      <c r="C11" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="39" t="s">
+      <c r="D11" s="35" t="s">
         <v>5</v>
       </c>
       <c r="E11" s="12"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="44"/>
+      <c r="A12" s="40"/>
       <c r="B12" s="20" t="s">
         <v>217</v>
       </c>
-      <c r="C12" s="39"/>
-      <c r="D12" s="39"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
       <c r="E12" s="12"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="44"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="21"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
       <c r="E13" s="12"/>
     </row>
     <row r="14" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="44"/>
+      <c r="A14" s="40"/>
       <c r="B14" s="21"/>
-      <c r="C14" s="39"/>
-      <c r="D14" s="39"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
       <c r="E14" s="12"/>
     </row>
     <row r="15" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="45" t="s">
+      <c r="A15" s="41" t="s">
         <v>214</v>
       </c>
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="29" t="s">
         <v>218</v>
       </c>
-      <c r="C15" s="85">
+      <c r="C15" s="66">
         <v>0</v>
       </c>
-      <c r="D15" s="40"/>
+      <c r="D15" s="36"/>
       <c r="E15" s="12"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="46"/>
+      <c r="A16" s="42"/>
       <c r="B16" s="22"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
       <c r="E16" s="12"/>
     </row>
-    <row r="17" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="47" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="43" t="s">
         <v>219</v>
       </c>
       <c r="B17" s="23" t="s">
         <v>220</v>
       </c>
-      <c r="C17" s="41" t="s">
+      <c r="C17" s="37" t="s">
         <v>200</v>
       </c>
-      <c r="D17" s="41" t="s">
+      <c r="D17" s="37" t="s">
         <v>204</v>
       </c>
       <c r="E17" s="12"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="71">
-        <v>42767</v>
-      </c>
-      <c r="B18" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="75">
-        <v>0</v>
-      </c>
-      <c r="D18" s="80">
-        <v>0</v>
-      </c>
-      <c r="E18" s="12"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="72">
-        <v>42767.010416666664</v>
-      </c>
-      <c r="B19" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="76">
-        <v>0</v>
-      </c>
-      <c r="D19" s="81">
-        <v>0</v>
-      </c>
-      <c r="E19" s="12"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="72">
-        <v>42767.020833333336</v>
-      </c>
-      <c r="B20" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="76">
-        <v>0</v>
-      </c>
-      <c r="D20" s="81">
-        <v>0</v>
-      </c>
-      <c r="E20" s="12"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="73">
-        <v>42767.03125</v>
-      </c>
-      <c r="B21" s="53" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="77">
-        <v>0</v>
-      </c>
-      <c r="D21" s="82">
-        <v>0</v>
-      </c>
-      <c r="E21" s="12"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="72">
-        <v>42767.041666666664</v>
-      </c>
-      <c r="B22" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" s="76">
-        <v>0</v>
-      </c>
-      <c r="D22" s="81">
-        <v>0</v>
-      </c>
-      <c r="E22" s="12"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="72">
-        <v>42767.052083333336</v>
-      </c>
-      <c r="B23" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" s="76">
-        <v>0</v>
-      </c>
-      <c r="D23" s="81">
-        <v>0</v>
-      </c>
-      <c r="E23" s="12"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="72">
-        <v>42767.0625</v>
-      </c>
-      <c r="B24" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="76">
-        <v>0</v>
-      </c>
-      <c r="D24" s="81">
-        <v>0</v>
-      </c>
-      <c r="E24" s="12"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="73">
-        <v>42767.072916666664</v>
-      </c>
-      <c r="B25" s="53" t="s">
-        <v>23</v>
-      </c>
-      <c r="C25" s="77">
-        <v>0</v>
-      </c>
-      <c r="D25" s="82">
-        <v>0</v>
-      </c>
-      <c r="E25" s="12"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="72">
-        <v>42767.083333333336</v>
-      </c>
-      <c r="B26" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="C26" s="76">
-        <v>0</v>
-      </c>
-      <c r="D26" s="81">
-        <v>0</v>
-      </c>
-      <c r="E26" s="12"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="72">
-        <v>42767.09375</v>
-      </c>
-      <c r="B27" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" s="76">
-        <v>0</v>
-      </c>
-      <c r="D27" s="81">
-        <v>0</v>
-      </c>
-      <c r="E27" s="12"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="72">
-        <v>42767.104166666664</v>
-      </c>
-      <c r="B28" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28" s="76">
-        <v>0</v>
-      </c>
-      <c r="D28" s="81">
-        <v>0</v>
-      </c>
-      <c r="E28" s="12"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="73">
-        <v>42767.114583333336</v>
-      </c>
-      <c r="B29" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29" s="77">
-        <v>0</v>
-      </c>
-      <c r="D29" s="82">
-        <v>0</v>
-      </c>
-      <c r="E29" s="12"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="72">
-        <v>42767.125</v>
-      </c>
-      <c r="B30" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="C30" s="76">
-        <v>0</v>
-      </c>
-      <c r="D30" s="81">
-        <v>0</v>
-      </c>
-      <c r="E30" s="12"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="72">
-        <v>42767.135416666664</v>
-      </c>
-      <c r="B31" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="C31" s="76">
-        <v>0</v>
-      </c>
-      <c r="D31" s="81">
-        <v>0</v>
-      </c>
-      <c r="E31" s="12"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="72">
-        <v>42767.145833333336</v>
-      </c>
-      <c r="B32" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="C32" s="76">
-        <v>0</v>
-      </c>
-      <c r="D32" s="81">
-        <v>0</v>
-      </c>
-      <c r="E32" s="12"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="73">
-        <v>42767.15625</v>
-      </c>
-      <c r="B33" s="53" t="s">
-        <v>39</v>
-      </c>
-      <c r="C33" s="77">
-        <v>0</v>
-      </c>
-      <c r="D33" s="82">
-        <v>0</v>
-      </c>
-      <c r="E33" s="12"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="72">
-        <v>42767.166666666664</v>
-      </c>
-      <c r="B34" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C34" s="76">
-        <v>0</v>
-      </c>
-      <c r="D34" s="81">
-        <v>0</v>
-      </c>
-      <c r="E34" s="12"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="72">
-        <v>42767.177083333336</v>
-      </c>
-      <c r="B35" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="C35" s="76">
-        <v>0</v>
-      </c>
-      <c r="D35" s="81">
-        <v>0</v>
-      </c>
-      <c r="E35" s="12"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="72">
-        <v>42767.1875</v>
-      </c>
-      <c r="B36" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="C36" s="76">
-        <v>0</v>
-      </c>
-      <c r="D36" s="81">
-        <v>0</v>
-      </c>
-      <c r="E36" s="12"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="73">
-        <v>42767.197916666664</v>
-      </c>
-      <c r="B37" s="53" t="s">
-        <v>47</v>
-      </c>
-      <c r="C37" s="77">
-        <v>0</v>
-      </c>
-      <c r="D37" s="82">
-        <v>0</v>
-      </c>
-      <c r="E37" s="12"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="72">
-        <v>42767.208333333336</v>
-      </c>
-      <c r="B38" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="C38" s="76">
-        <v>0</v>
-      </c>
-      <c r="D38" s="81">
-        <v>0</v>
-      </c>
-      <c r="E38" s="12"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="72">
-        <v>42767.21875</v>
-      </c>
-      <c r="B39" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="C39" s="76">
-        <v>0</v>
-      </c>
-      <c r="D39" s="81">
-        <v>0</v>
-      </c>
-      <c r="E39" s="12"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="72">
-        <v>42767.229166666664</v>
-      </c>
-      <c r="B40" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="C40" s="76">
-        <v>0</v>
-      </c>
-      <c r="D40" s="81">
-        <v>0</v>
-      </c>
-      <c r="E40" s="12"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="73">
-        <v>42767.239583333336</v>
-      </c>
-      <c r="B41" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="C41" s="77">
-        <v>0</v>
-      </c>
-      <c r="D41" s="82">
-        <v>0</v>
-      </c>
-      <c r="E41" s="12"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="72">
-        <v>42767.25</v>
-      </c>
-      <c r="B42" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="C42" s="76">
-        <v>0</v>
-      </c>
-      <c r="D42" s="81">
-        <v>0</v>
-      </c>
-      <c r="E42" s="12"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="72">
-        <v>42767.260416666664</v>
-      </c>
-      <c r="B43" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="C43" s="76">
-        <v>0</v>
-      </c>
-      <c r="D43" s="81">
-        <v>0</v>
-      </c>
-      <c r="E43" s="12"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="72">
-        <v>42767.270833333336</v>
-      </c>
-      <c r="B44" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="C44" s="76">
-        <v>0</v>
-      </c>
-      <c r="D44" s="81">
-        <v>0</v>
-      </c>
-      <c r="E44" s="12"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="73">
-        <v>42767.28125</v>
-      </c>
-      <c r="B45" s="53" t="s">
-        <v>63</v>
-      </c>
-      <c r="C45" s="77">
-        <v>0</v>
-      </c>
-      <c r="D45" s="82">
-        <v>0</v>
-      </c>
-      <c r="E45" s="12"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="72">
-        <v>42767.291666666664</v>
-      </c>
-      <c r="B46" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="C46" s="76">
-        <v>0</v>
-      </c>
-      <c r="D46" s="81">
-        <v>0</v>
-      </c>
-      <c r="E46" s="12"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="72">
-        <v>42767.302083333336</v>
-      </c>
-      <c r="B47" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="C47" s="76">
-        <v>0</v>
-      </c>
-      <c r="D47" s="81">
-        <v>0</v>
-      </c>
-      <c r="E47" s="12"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="72">
-        <v>42767.3125</v>
-      </c>
-      <c r="B48" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="C48" s="76">
-        <v>0</v>
-      </c>
-      <c r="D48" s="81">
-        <v>0</v>
-      </c>
-      <c r="E48" s="12"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" s="73">
-        <v>42767.322916666664</v>
-      </c>
-      <c r="B49" s="53" t="s">
-        <v>71</v>
-      </c>
-      <c r="C49" s="77">
-        <v>0</v>
-      </c>
-      <c r="D49" s="82">
-        <v>0</v>
-      </c>
-      <c r="E49" s="12"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" s="72">
-        <v>42767.333333333336</v>
-      </c>
-      <c r="B50" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="C50" s="76">
-        <v>0</v>
-      </c>
-      <c r="D50" s="81">
-        <v>0</v>
-      </c>
-      <c r="E50" s="12"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" s="72">
-        <v>42767.34375</v>
-      </c>
-      <c r="B51" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="C51" s="76">
-        <v>0</v>
-      </c>
-      <c r="D51" s="81">
-        <v>0</v>
-      </c>
-      <c r="E51" s="12"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52" s="72">
-        <v>42767.354166666664</v>
-      </c>
-      <c r="B52" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="C52" s="76">
-        <v>0</v>
-      </c>
-      <c r="D52" s="81">
-        <v>0</v>
-      </c>
-      <c r="E52" s="12"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" s="73">
-        <v>42767.364583333336</v>
-      </c>
-      <c r="B53" s="53" t="s">
-        <v>79</v>
-      </c>
-      <c r="C53" s="77">
-        <v>0</v>
-      </c>
-      <c r="D53" s="82">
-        <v>0</v>
-      </c>
-      <c r="E53" s="12"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54" s="72">
-        <v>42767.375</v>
-      </c>
-      <c r="B54" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="C54" s="76">
-        <v>0</v>
-      </c>
-      <c r="D54" s="81">
-        <v>0</v>
-      </c>
-      <c r="E54" s="12"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55" s="72">
-        <v>42767.385416666664</v>
-      </c>
-      <c r="B55" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="C55" s="76">
-        <v>0</v>
-      </c>
-      <c r="D55" s="81">
-        <v>0</v>
-      </c>
-      <c r="E55" s="12"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56" s="72">
-        <v>42767.395833333336</v>
-      </c>
-      <c r="B56" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="C56" s="76">
-        <v>0</v>
-      </c>
-      <c r="D56" s="81">
-        <v>0</v>
-      </c>
-      <c r="E56" s="12"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57" s="73">
-        <v>42767.40625</v>
-      </c>
-      <c r="B57" s="53" t="s">
-        <v>87</v>
-      </c>
-      <c r="C57" s="77">
-        <v>0</v>
-      </c>
-      <c r="D57" s="82">
-        <v>0</v>
-      </c>
-      <c r="E57" s="12"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58" s="72">
-        <v>42767.416666666664</v>
-      </c>
-      <c r="B58" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="C58" s="76">
-        <v>0</v>
-      </c>
-      <c r="D58" s="81">
-        <v>0</v>
-      </c>
-      <c r="E58" s="12"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59" s="72">
-        <v>42767.427083333336</v>
-      </c>
-      <c r="B59" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="C59" s="76">
-        <v>0</v>
-      </c>
-      <c r="D59" s="81">
-        <v>0</v>
-      </c>
-      <c r="E59" s="12"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60" s="72">
-        <v>42767.4375</v>
-      </c>
-      <c r="B60" s="24" t="s">
-        <v>93</v>
-      </c>
-      <c r="C60" s="76">
-        <v>0</v>
-      </c>
-      <c r="D60" s="81">
-        <v>0</v>
-      </c>
-      <c r="E60" s="12"/>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61" s="73">
-        <v>42767.447916666664</v>
-      </c>
-      <c r="B61" s="53" t="s">
-        <v>95</v>
-      </c>
-      <c r="C61" s="77">
-        <v>0</v>
-      </c>
-      <c r="D61" s="82">
-        <v>0</v>
-      </c>
-      <c r="E61" s="12"/>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62" s="72">
-        <v>42767.458333333336</v>
-      </c>
-      <c r="B62" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="C62" s="76">
-        <v>0</v>
-      </c>
-      <c r="D62" s="81">
-        <v>0</v>
-      </c>
-      <c r="E62" s="12"/>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63" s="72">
-        <v>42767.46875</v>
-      </c>
-      <c r="B63" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="C63" s="76">
-        <v>0</v>
-      </c>
-      <c r="D63" s="81">
-        <v>0</v>
-      </c>
-      <c r="E63" s="12"/>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64" s="72">
-        <v>42767.479166666664</v>
-      </c>
-      <c r="B64" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="C64" s="76">
-        <v>0</v>
-      </c>
-      <c r="D64" s="81">
-        <v>0</v>
-      </c>
-      <c r="E64" s="12"/>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A65" s="73">
-        <v>42767.489583333336</v>
-      </c>
-      <c r="B65" s="53" t="s">
-        <v>103</v>
-      </c>
-      <c r="C65" s="77">
-        <v>0</v>
-      </c>
-      <c r="D65" s="82">
-        <v>0</v>
-      </c>
-      <c r="E65" s="12"/>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A66" s="72">
-        <v>42767.5</v>
-      </c>
-      <c r="B66" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="C66" s="76">
-        <v>0</v>
-      </c>
-      <c r="D66" s="81">
-        <v>0</v>
-      </c>
-      <c r="E66" s="12"/>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A67" s="72">
-        <v>42767.510416666664</v>
-      </c>
-      <c r="B67" s="24" t="s">
-        <v>107</v>
-      </c>
-      <c r="C67" s="76">
-        <v>0</v>
-      </c>
-      <c r="D67" s="81">
-        <v>0</v>
-      </c>
-      <c r="E67" s="12"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A68" s="72">
-        <v>42767.520833333336</v>
-      </c>
-      <c r="B68" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="C68" s="76">
-        <v>0</v>
-      </c>
-      <c r="D68" s="81">
-        <v>0</v>
-      </c>
-      <c r="E68" s="12"/>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A69" s="73">
-        <v>42767.53125</v>
-      </c>
-      <c r="B69" s="53" t="s">
-        <v>111</v>
-      </c>
-      <c r="C69" s="77">
-        <v>0</v>
-      </c>
-      <c r="D69" s="82">
-        <v>0</v>
-      </c>
-      <c r="E69" s="12"/>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A70" s="72">
-        <v>42767.541666666664</v>
-      </c>
-      <c r="B70" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="C70" s="76">
-        <v>0</v>
-      </c>
-      <c r="D70" s="81">
-        <v>0</v>
-      </c>
-      <c r="E70" s="12"/>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A71" s="72">
-        <v>42767.552083333336</v>
-      </c>
-      <c r="B71" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="C71" s="76">
-        <v>0</v>
-      </c>
-      <c r="D71" s="81">
-        <v>0</v>
-      </c>
-      <c r="E71" s="12"/>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A72" s="72">
-        <v>42767.5625</v>
-      </c>
-      <c r="B72" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="C72" s="76">
-        <v>0</v>
-      </c>
-      <c r="D72" s="81">
-        <v>0</v>
-      </c>
-      <c r="E72" s="12"/>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A73" s="73">
-        <v>42767.572916666664</v>
-      </c>
-      <c r="B73" s="53" t="s">
-        <v>119</v>
-      </c>
-      <c r="C73" s="77">
-        <v>0</v>
-      </c>
-      <c r="D73" s="82">
-        <v>0</v>
-      </c>
-      <c r="E73" s="12"/>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A74" s="72">
-        <v>42767.583333333336</v>
-      </c>
-      <c r="B74" s="24" t="s">
-        <v>121</v>
-      </c>
-      <c r="C74" s="76">
-        <v>0</v>
-      </c>
-      <c r="D74" s="81">
-        <v>0</v>
-      </c>
-      <c r="E74" s="12"/>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A75" s="72">
-        <v>42767.59375</v>
-      </c>
-      <c r="B75" s="24" t="s">
-        <v>123</v>
-      </c>
-      <c r="C75" s="76">
-        <v>0</v>
-      </c>
-      <c r="D75" s="81">
-        <v>0</v>
-      </c>
-      <c r="E75" s="12"/>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A76" s="72">
-        <v>42767.604166666664</v>
-      </c>
-      <c r="B76" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="C76" s="76">
-        <v>0</v>
-      </c>
-      <c r="D76" s="81">
-        <v>0</v>
-      </c>
-      <c r="E76" s="12"/>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A77" s="73">
-        <v>42767.614583333336</v>
-      </c>
-      <c r="B77" s="53" t="s">
-        <v>127</v>
-      </c>
-      <c r="C77" s="77">
-        <v>0</v>
-      </c>
-      <c r="D77" s="82">
-        <v>0</v>
-      </c>
-      <c r="E77" s="12"/>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A78" s="72">
-        <v>42767.625</v>
-      </c>
-      <c r="B78" s="24" t="s">
-        <v>129</v>
-      </c>
-      <c r="C78" s="76">
-        <v>0</v>
-      </c>
-      <c r="D78" s="81">
-        <v>0</v>
-      </c>
-      <c r="E78" s="12"/>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A79" s="72">
-        <v>42767.635416666664</v>
-      </c>
-      <c r="B79" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="C79" s="76">
-        <v>0</v>
-      </c>
-      <c r="D79" s="81">
-        <v>0</v>
-      </c>
-      <c r="E79" s="12"/>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A80" s="72">
-        <v>42767.645833333336</v>
-      </c>
-      <c r="B80" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="C80" s="76">
-        <v>0</v>
-      </c>
-      <c r="D80" s="81">
-        <v>0</v>
-      </c>
-      <c r="E80" s="12"/>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A81" s="73">
-        <v>42767.65625</v>
-      </c>
-      <c r="B81" s="53" t="s">
-        <v>135</v>
-      </c>
-      <c r="C81" s="77">
-        <v>0</v>
-      </c>
-      <c r="D81" s="81">
-        <v>0</v>
-      </c>
-      <c r="E81" s="12"/>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A82" s="72">
-        <v>42767.666666666664</v>
-      </c>
-      <c r="B82" s="24" t="s">
-        <v>137</v>
-      </c>
-      <c r="C82" s="76">
-        <v>0</v>
-      </c>
-      <c r="D82" s="82">
-        <v>0</v>
-      </c>
-      <c r="E82" s="12"/>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A83" s="72">
-        <v>42767.677083333336</v>
-      </c>
-      <c r="B83" s="24" t="s">
-        <v>139</v>
-      </c>
-      <c r="C83" s="76">
-        <v>0</v>
-      </c>
-      <c r="D83" s="81">
-        <v>0</v>
-      </c>
-      <c r="E83" s="12"/>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A84" s="72">
-        <v>42767.6875</v>
-      </c>
-      <c r="B84" s="24" t="s">
-        <v>141</v>
-      </c>
-      <c r="C84" s="76">
-        <v>0</v>
-      </c>
-      <c r="D84" s="81">
-        <v>0</v>
-      </c>
-      <c r="E84" s="12"/>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A85" s="73">
-        <v>42767.697916666664</v>
-      </c>
-      <c r="B85" s="53" t="s">
-        <v>143</v>
-      </c>
-      <c r="C85" s="77">
-        <v>0</v>
-      </c>
-      <c r="D85" s="81">
-        <v>0</v>
-      </c>
-      <c r="E85" s="12"/>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A86" s="72">
-        <v>42767.708333333336</v>
-      </c>
-      <c r="B86" s="24" t="s">
-        <v>145</v>
-      </c>
-      <c r="C86" s="76">
-        <v>0</v>
-      </c>
-      <c r="D86" s="81">
-        <v>0</v>
-      </c>
-      <c r="E86" s="12"/>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A87" s="72">
-        <v>42767.71875</v>
-      </c>
-      <c r="B87" s="24" t="s">
-        <v>147</v>
-      </c>
-      <c r="C87" s="76">
-        <v>0</v>
-      </c>
-      <c r="D87" s="82">
-        <v>0</v>
-      </c>
-      <c r="E87" s="12"/>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A88" s="72">
-        <v>42767.729166666664</v>
-      </c>
-      <c r="B88" s="24" t="s">
-        <v>149</v>
-      </c>
-      <c r="C88" s="76">
-        <v>0</v>
-      </c>
-      <c r="D88" s="81">
-        <v>0</v>
-      </c>
-      <c r="E88" s="12"/>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A89" s="73">
-        <v>42767.739583333336</v>
-      </c>
-      <c r="B89" s="53" t="s">
-        <v>151</v>
-      </c>
-      <c r="C89" s="77">
-        <v>0</v>
-      </c>
-      <c r="D89" s="81">
-        <v>0</v>
-      </c>
-      <c r="E89" s="12"/>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A90" s="72">
-        <v>42767.75</v>
-      </c>
-      <c r="B90" s="24" t="s">
-        <v>153</v>
-      </c>
-      <c r="C90" s="76">
-        <v>0</v>
-      </c>
-      <c r="D90" s="81">
-        <v>0</v>
-      </c>
-      <c r="E90" s="12"/>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A91" s="72">
-        <v>42767.760416666664</v>
-      </c>
-      <c r="B91" s="24" t="s">
-        <v>155</v>
-      </c>
-      <c r="C91" s="76">
-        <v>0</v>
-      </c>
-      <c r="D91" s="81">
-        <v>0</v>
-      </c>
-      <c r="E91" s="12"/>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A92" s="72">
-        <v>42767.770833333336</v>
-      </c>
-      <c r="B92" s="24" t="s">
-        <v>157</v>
-      </c>
-      <c r="C92" s="76">
-        <v>0</v>
-      </c>
-      <c r="D92" s="82">
-        <v>0</v>
-      </c>
-      <c r="E92" s="12"/>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A93" s="73">
-        <v>42767.78125</v>
-      </c>
-      <c r="B93" s="53" t="s">
-        <v>159</v>
-      </c>
-      <c r="C93" s="77">
-        <v>0</v>
-      </c>
-      <c r="D93" s="81">
-        <v>0</v>
-      </c>
-      <c r="E93" s="12"/>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A94" s="72">
-        <v>42767.791666666664</v>
-      </c>
-      <c r="B94" s="24" t="s">
-        <v>161</v>
-      </c>
-      <c r="C94" s="76">
-        <v>0</v>
-      </c>
-      <c r="D94" s="81">
-        <v>0</v>
-      </c>
-      <c r="E94" s="12"/>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A95" s="72">
-        <v>42767.802083333336</v>
-      </c>
-      <c r="B95" s="24" t="s">
-        <v>163</v>
-      </c>
-      <c r="C95" s="76">
-        <v>0</v>
-      </c>
-      <c r="D95" s="81">
-        <v>0</v>
-      </c>
-      <c r="E95" s="12"/>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A96" s="72">
-        <v>42767.8125</v>
-      </c>
-      <c r="B96" s="24" t="s">
-        <v>165</v>
-      </c>
-      <c r="C96" s="76">
-        <v>0</v>
-      </c>
-      <c r="D96" s="81">
-        <v>0</v>
-      </c>
-      <c r="E96" s="12"/>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A97" s="73">
-        <v>42767.822916666664</v>
-      </c>
-      <c r="B97" s="53" t="s">
-        <v>167</v>
-      </c>
-      <c r="C97" s="77">
-        <v>0</v>
-      </c>
-      <c r="D97" s="82">
-        <v>0</v>
-      </c>
-      <c r="E97" s="12"/>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A98" s="72">
-        <v>42767.833333333336</v>
-      </c>
-      <c r="B98" s="24" t="s">
-        <v>169</v>
-      </c>
-      <c r="C98" s="76">
-        <v>0</v>
-      </c>
-      <c r="D98" s="81">
-        <v>0</v>
-      </c>
-      <c r="E98" s="12"/>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A99" s="72">
-        <v>42767.84375</v>
-      </c>
-      <c r="B99" s="24" t="s">
-        <v>171</v>
-      </c>
-      <c r="C99" s="76">
-        <v>0</v>
-      </c>
-      <c r="D99" s="81">
-        <v>0</v>
-      </c>
-      <c r="E99" s="12"/>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A100" s="72">
-        <v>42767.854166666664</v>
-      </c>
-      <c r="B100" s="24" t="s">
-        <v>173</v>
-      </c>
-      <c r="C100" s="76">
-        <v>0</v>
-      </c>
-      <c r="D100" s="81">
-        <v>0</v>
-      </c>
-      <c r="E100" s="12"/>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A101" s="73">
-        <v>42767.864583333336</v>
-      </c>
-      <c r="B101" s="53" t="s">
-        <v>175</v>
-      </c>
-      <c r="C101" s="77">
-        <v>0</v>
-      </c>
-      <c r="D101" s="81">
-        <v>0</v>
-      </c>
-      <c r="E101" s="12"/>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A102" s="72">
-        <v>42767.875</v>
-      </c>
-      <c r="B102" s="24" t="s">
-        <v>177</v>
-      </c>
-      <c r="C102" s="76">
-        <v>0</v>
-      </c>
-      <c r="D102" s="81">
-        <v>0</v>
-      </c>
-      <c r="E102" s="12"/>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A103" s="72">
-        <v>42767.885416666664</v>
-      </c>
-      <c r="B103" s="24" t="s">
-        <v>179</v>
-      </c>
-      <c r="C103" s="76">
-        <v>0</v>
-      </c>
-      <c r="D103" s="81">
-        <v>0</v>
-      </c>
-      <c r="E103" s="12"/>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A104" s="72">
-        <v>42767.895833333336</v>
-      </c>
-      <c r="B104" s="24" t="s">
-        <v>181</v>
-      </c>
-      <c r="C104" s="76">
-        <v>0</v>
-      </c>
-      <c r="D104" s="81">
-        <v>0</v>
-      </c>
-      <c r="E104" s="12"/>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A105" s="73">
-        <v>42767.90625</v>
-      </c>
-      <c r="B105" s="53" t="s">
-        <v>183</v>
-      </c>
-      <c r="C105" s="77">
-        <v>0</v>
-      </c>
-      <c r="D105" s="82">
-        <v>0</v>
-      </c>
-      <c r="E105" s="12"/>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A106" s="72">
-        <v>42767.916666666664</v>
-      </c>
-      <c r="B106" s="24" t="s">
-        <v>185</v>
-      </c>
-      <c r="C106" s="76">
-        <v>0</v>
-      </c>
-      <c r="D106" s="81">
-        <v>0</v>
-      </c>
-      <c r="E106" s="12"/>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A107" s="72">
-        <v>42767.927083333336</v>
-      </c>
-      <c r="B107" s="24" t="s">
-        <v>187</v>
-      </c>
-      <c r="C107" s="76">
-        <v>0</v>
-      </c>
-      <c r="D107" s="81">
-        <v>0</v>
-      </c>
-      <c r="E107" s="12"/>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A108" s="72">
-        <v>42767.9375</v>
-      </c>
-      <c r="B108" s="24" t="s">
-        <v>189</v>
-      </c>
-      <c r="C108" s="76">
-        <v>0</v>
-      </c>
-      <c r="D108" s="81">
-        <v>0</v>
-      </c>
-      <c r="E108" s="12"/>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A109" s="73">
-        <v>42767.947916666664</v>
-      </c>
-      <c r="B109" s="53" t="s">
-        <v>191</v>
-      </c>
-      <c r="C109" s="77">
-        <v>0</v>
-      </c>
-      <c r="D109" s="82">
-        <v>0</v>
-      </c>
-      <c r="E109" s="12"/>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A110" s="72">
-        <v>42767.958333333336</v>
-      </c>
-      <c r="B110" s="24" t="s">
-        <v>193</v>
-      </c>
-      <c r="C110" s="76">
-        <v>0</v>
-      </c>
-      <c r="D110" s="81">
-        <v>0</v>
-      </c>
-      <c r="E110" s="12"/>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A111" s="72">
-        <v>42767.96875</v>
-      </c>
-      <c r="B111" s="24" t="s">
-        <v>195</v>
-      </c>
-      <c r="C111" s="76">
-        <v>0</v>
-      </c>
-      <c r="D111" s="81">
-        <v>0</v>
-      </c>
-      <c r="E111" s="12"/>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A112" s="72">
-        <v>42767.979166666664</v>
-      </c>
-      <c r="B112" s="24" t="s">
-        <v>197</v>
-      </c>
-      <c r="C112" s="76">
-        <v>0</v>
-      </c>
-      <c r="D112" s="81">
-        <v>0</v>
-      </c>
-      <c r="E112" s="12"/>
-    </row>
-    <row r="113" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="74">
-        <v>42767.989583333336</v>
-      </c>
-      <c r="B113" s="33" t="s">
-        <v>199</v>
-      </c>
-      <c r="C113" s="78">
-        <v>0</v>
-      </c>
-      <c r="D113" s="83">
-        <v>0</v>
-      </c>
-      <c r="E113" s="12"/>
-    </row>
-    <row r="114" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="51"/>
-      <c r="B114" s="27" t="s">
-        <v>221</v>
-      </c>
-      <c r="C114" s="79">
-        <v>0</v>
-      </c>
-      <c r="D114" s="84"/>
-      <c r="E114" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -3319,993 +1782,993 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="38" t="s">
         <v>222</v>
       </c>
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="50" t="s">
         <v>207</v>
       </c>
-      <c r="C1" s="54"/>
+      <c r="C1" s="49"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="24" t="s">
         <v>206</v>
       </c>
-      <c r="B2" s="65" t="s">
+      <c r="B2" s="60" t="s">
         <v>208</v>
       </c>
       <c r="C2" s="13"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="17"/>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="51" t="s">
         <v>209</v>
       </c>
       <c r="C3" s="13"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="17"/>
-      <c r="B4" s="57" t="s">
+      <c r="B4" s="52" t="s">
         <v>210</v>
       </c>
       <c r="C4" s="14"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="17"/>
-      <c r="B5" s="57" t="s">
+      <c r="B5" s="52" t="s">
         <v>211</v>
       </c>
       <c r="C5" s="14"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="17"/>
-      <c r="B6" s="58"/>
+      <c r="B6" s="53"/>
       <c r="C6" s="14"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="17"/>
-      <c r="B7" s="57" t="s">
+      <c r="B7" s="52" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="14"/>
     </row>
     <row r="8" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="29"/>
-      <c r="B8" s="66" t="s">
+      <c r="A8" s="27"/>
+      <c r="B8" s="61" t="s">
         <v>212</v>
       </c>
       <c r="C8" s="13"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="39" t="s">
         <v>213</v>
       </c>
-      <c r="B9" s="59" t="s">
+      <c r="B9" s="54" t="s">
         <v>215</v>
       </c>
       <c r="C9" s="12"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="44"/>
-      <c r="B10" s="59" t="s">
+      <c r="A10" s="40"/>
+      <c r="B10" s="54" t="s">
         <v>217</v>
       </c>
       <c r="C10" s="12"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="44"/>
-      <c r="B11" s="59" t="s">
+      <c r="A11" s="40"/>
+      <c r="B11" s="54" t="s">
         <v>216</v>
       </c>
       <c r="C11" s="12"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="44"/>
-      <c r="B12" s="59" t="s">
+      <c r="A12" s="40"/>
+      <c r="B12" s="54" t="s">
         <v>217</v>
       </c>
       <c r="C12" s="12"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="44"/>
-      <c r="B13" s="60"/>
+      <c r="A13" s="40"/>
+      <c r="B13" s="55"/>
       <c r="C13" s="12"/>
     </row>
     <row r="14" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="44"/>
-      <c r="B14" s="60"/>
+      <c r="A14" s="40"/>
+      <c r="B14" s="55"/>
       <c r="C14" s="12"/>
     </row>
     <row r="15" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="45" t="s">
+      <c r="A15" s="41" t="s">
         <v>214</v>
       </c>
-      <c r="B15" s="67" t="s">
+      <c r="B15" s="62" t="s">
         <v>218</v>
       </c>
       <c r="C15" s="15"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="46"/>
-      <c r="B16" s="61"/>
+      <c r="A16" s="42"/>
+      <c r="B16" s="56"/>
       <c r="C16" s="15"/>
     </row>
     <row r="17" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="47" t="s">
+      <c r="A17" s="43" t="s">
         <v>219</v>
       </c>
-      <c r="B17" s="62" t="s">
+      <c r="B17" s="57" t="s">
         <v>220</v>
       </c>
       <c r="C17" s="15"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="48" t="s">
+      <c r="A18" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="68" t="s">
+      <c r="B18" s="63" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="12"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="49" t="s">
+      <c r="A19" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="63" t="s">
+      <c r="B19" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C19" s="12"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="49" t="s">
+      <c r="A20" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="63" t="s">
+      <c r="B20" s="58" t="s">
         <v>13</v>
       </c>
       <c r="C20" s="12"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="52" t="s">
+      <c r="A21" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="70" t="s">
+      <c r="B21" s="65" t="s">
         <v>15</v>
       </c>
       <c r="C21" s="12"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="49" t="s">
+      <c r="A22" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="63" t="s">
+      <c r="B22" s="58" t="s">
         <v>17</v>
       </c>
       <c r="C22" s="12"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="49" t="s">
+      <c r="A23" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="63" t="s">
+      <c r="B23" s="58" t="s">
         <v>19</v>
       </c>
       <c r="C23" s="12"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="49" t="s">
+      <c r="A24" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="63" t="s">
+      <c r="B24" s="58" t="s">
         <v>21</v>
       </c>
       <c r="C24" s="12"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="52" t="s">
+      <c r="A25" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="70" t="s">
+      <c r="B25" s="65" t="s">
         <v>23</v>
       </c>
       <c r="C25" s="12"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="49" t="s">
+      <c r="A26" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="63" t="s">
+      <c r="B26" s="58" t="s">
         <v>25</v>
       </c>
       <c r="C26" s="12"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="49" t="s">
+      <c r="A27" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="63" t="s">
+      <c r="B27" s="58" t="s">
         <v>27</v>
       </c>
       <c r="C27" s="12"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="49" t="s">
+      <c r="A28" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="63" t="s">
+      <c r="B28" s="58" t="s">
         <v>29</v>
       </c>
       <c r="C28" s="12"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="52" t="s">
+      <c r="A29" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="B29" s="70" t="s">
+      <c r="B29" s="65" t="s">
         <v>31</v>
       </c>
       <c r="C29" s="12"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="49" t="s">
+      <c r="A30" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="63" t="s">
+      <c r="B30" s="58" t="s">
         <v>33</v>
       </c>
       <c r="C30" s="12"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="49" t="s">
+      <c r="A31" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="63" t="s">
+      <c r="B31" s="58" t="s">
         <v>35</v>
       </c>
       <c r="C31" s="12"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="49" t="s">
+      <c r="A32" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="63" t="s">
+      <c r="B32" s="58" t="s">
         <v>37</v>
       </c>
       <c r="C32" s="12"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="52" t="s">
+      <c r="A33" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="70" t="s">
+      <c r="B33" s="65" t="s">
         <v>39</v>
       </c>
       <c r="C33" s="12"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="49" t="s">
+      <c r="A34" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="B34" s="63" t="s">
+      <c r="B34" s="58" t="s">
         <v>41</v>
       </c>
       <c r="C34" s="12"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="49" t="s">
+      <c r="A35" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="B35" s="63" t="s">
+      <c r="B35" s="58" t="s">
         <v>43</v>
       </c>
       <c r="C35" s="12"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="49" t="s">
+      <c r="A36" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="B36" s="63" t="s">
+      <c r="B36" s="58" t="s">
         <v>45</v>
       </c>
       <c r="C36" s="12"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="52" t="s">
+      <c r="A37" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="B37" s="70" t="s">
+      <c r="B37" s="65" t="s">
         <v>47</v>
       </c>
       <c r="C37" s="12"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="49" t="s">
+      <c r="A38" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="B38" s="63" t="s">
+      <c r="B38" s="58" t="s">
         <v>49</v>
       </c>
       <c r="C38" s="12"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="49" t="s">
+      <c r="A39" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="B39" s="63" t="s">
+      <c r="B39" s="58" t="s">
         <v>51</v>
       </c>
       <c r="C39" s="12"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="49" t="s">
+      <c r="A40" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="B40" s="63" t="s">
+      <c r="B40" s="58" t="s">
         <v>53</v>
       </c>
       <c r="C40" s="12"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="52" t="s">
+      <c r="A41" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="B41" s="70" t="s">
+      <c r="B41" s="65" t="s">
         <v>55</v>
       </c>
       <c r="C41" s="12"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="49" t="s">
+      <c r="A42" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="B42" s="63" t="s">
+      <c r="B42" s="58" t="s">
         <v>57</v>
       </c>
       <c r="C42" s="12"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="49" t="s">
+      <c r="A43" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="B43" s="63" t="s">
+      <c r="B43" s="58" t="s">
         <v>59</v>
       </c>
       <c r="C43" s="12"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="49" t="s">
+      <c r="A44" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="B44" s="63" t="s">
+      <c r="B44" s="58" t="s">
         <v>61</v>
       </c>
       <c r="C44" s="12"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="52" t="s">
+      <c r="A45" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="B45" s="70" t="s">
+      <c r="B45" s="65" t="s">
         <v>63</v>
       </c>
       <c r="C45" s="12"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="49" t="s">
+      <c r="A46" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="B46" s="63" t="s">
+      <c r="B46" s="58" t="s">
         <v>65</v>
       </c>
       <c r="C46" s="12"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="49" t="s">
+      <c r="A47" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="B47" s="63" t="s">
+      <c r="B47" s="58" t="s">
         <v>67</v>
       </c>
       <c r="C47" s="12"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="49" t="s">
+      <c r="A48" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="B48" s="63" t="s">
+      <c r="B48" s="58" t="s">
         <v>69</v>
       </c>
       <c r="C48" s="12"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="52" t="s">
+      <c r="A49" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="B49" s="70" t="s">
+      <c r="B49" s="65" t="s">
         <v>71</v>
       </c>
       <c r="C49" s="12"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="49" t="s">
+      <c r="A50" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="B50" s="63" t="s">
+      <c r="B50" s="58" t="s">
         <v>73</v>
       </c>
       <c r="C50" s="12"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="49" t="s">
+      <c r="A51" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="B51" s="63" t="s">
+      <c r="B51" s="58" t="s">
         <v>75</v>
       </c>
       <c r="C51" s="12"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="49" t="s">
+      <c r="A52" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="B52" s="63" t="s">
+      <c r="B52" s="58" t="s">
         <v>77</v>
       </c>
       <c r="C52" s="12"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="52" t="s">
+      <c r="A53" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="B53" s="70" t="s">
+      <c r="B53" s="65" t="s">
         <v>79</v>
       </c>
       <c r="C53" s="12"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" s="49" t="s">
+      <c r="A54" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="B54" s="63" t="s">
+      <c r="B54" s="58" t="s">
         <v>81</v>
       </c>
       <c r="C54" s="12"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="49" t="s">
+      <c r="A55" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="B55" s="63" t="s">
+      <c r="B55" s="58" t="s">
         <v>83</v>
       </c>
       <c r="C55" s="12"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" s="49" t="s">
+      <c r="A56" s="45" t="s">
         <v>84</v>
       </c>
-      <c r="B56" s="63" t="s">
+      <c r="B56" s="58" t="s">
         <v>85</v>
       </c>
       <c r="C56" s="12"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="52" t="s">
+      <c r="A57" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="B57" s="70" t="s">
+      <c r="B57" s="65" t="s">
         <v>87</v>
       </c>
       <c r="C57" s="12"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" s="49" t="s">
+      <c r="A58" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="B58" s="63" t="s">
+      <c r="B58" s="58" t="s">
         <v>89</v>
       </c>
       <c r="C58" s="12"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" s="49" t="s">
+      <c r="A59" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="B59" s="63" t="s">
+      <c r="B59" s="58" t="s">
         <v>91</v>
       </c>
       <c r="C59" s="12"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" s="49" t="s">
+      <c r="A60" s="45" t="s">
         <v>92</v>
       </c>
-      <c r="B60" s="63" t="s">
+      <c r="B60" s="58" t="s">
         <v>93</v>
       </c>
       <c r="C60" s="12"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" s="52" t="s">
+      <c r="A61" s="48" t="s">
         <v>94</v>
       </c>
-      <c r="B61" s="70" t="s">
+      <c r="B61" s="65" t="s">
         <v>95</v>
       </c>
       <c r="C61" s="12"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" s="49" t="s">
+      <c r="A62" s="45" t="s">
         <v>96</v>
       </c>
-      <c r="B62" s="63" t="s">
+      <c r="B62" s="58" t="s">
         <v>97</v>
       </c>
       <c r="C62" s="12"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" s="49" t="s">
+      <c r="A63" s="45" t="s">
         <v>98</v>
       </c>
-      <c r="B63" s="63" t="s">
+      <c r="B63" s="58" t="s">
         <v>99</v>
       </c>
       <c r="C63" s="12"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" s="49" t="s">
+      <c r="A64" s="45" t="s">
         <v>100</v>
       </c>
-      <c r="B64" s="63" t="s">
+      <c r="B64" s="58" t="s">
         <v>101</v>
       </c>
       <c r="C64" s="12"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65" s="52" t="s">
+      <c r="A65" s="48" t="s">
         <v>102</v>
       </c>
-      <c r="B65" s="70" t="s">
+      <c r="B65" s="65" t="s">
         <v>103</v>
       </c>
       <c r="C65" s="12"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" s="49" t="s">
+      <c r="A66" s="45" t="s">
         <v>104</v>
       </c>
-      <c r="B66" s="63" t="s">
+      <c r="B66" s="58" t="s">
         <v>105</v>
       </c>
       <c r="C66" s="12"/>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" s="49" t="s">
+      <c r="A67" s="45" t="s">
         <v>106</v>
       </c>
-      <c r="B67" s="63" t="s">
+      <c r="B67" s="58" t="s">
         <v>107</v>
       </c>
       <c r="C67" s="12"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" s="49" t="s">
+      <c r="A68" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="B68" s="63" t="s">
+      <c r="B68" s="58" t="s">
         <v>109</v>
       </c>
       <c r="C68" s="12"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69" s="52" t="s">
+      <c r="A69" s="48" t="s">
         <v>110</v>
       </c>
-      <c r="B69" s="70" t="s">
+      <c r="B69" s="65" t="s">
         <v>111</v>
       </c>
       <c r="C69" s="12"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" s="49" t="s">
+      <c r="A70" s="45" t="s">
         <v>112</v>
       </c>
-      <c r="B70" s="63" t="s">
+      <c r="B70" s="58" t="s">
         <v>113</v>
       </c>
       <c r="C70" s="12"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" s="49" t="s">
+      <c r="A71" s="45" t="s">
         <v>114</v>
       </c>
-      <c r="B71" s="63" t="s">
+      <c r="B71" s="58" t="s">
         <v>115</v>
       </c>
       <c r="C71" s="12"/>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" s="49" t="s">
+      <c r="A72" s="45" t="s">
         <v>116</v>
       </c>
-      <c r="B72" s="63" t="s">
+      <c r="B72" s="58" t="s">
         <v>117</v>
       </c>
       <c r="C72" s="12"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73" s="52" t="s">
+      <c r="A73" s="48" t="s">
         <v>118</v>
       </c>
-      <c r="B73" s="70" t="s">
+      <c r="B73" s="65" t="s">
         <v>119</v>
       </c>
       <c r="C73" s="12"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74" s="49" t="s">
+      <c r="A74" s="45" t="s">
         <v>120</v>
       </c>
-      <c r="B74" s="63" t="s">
+      <c r="B74" s="58" t="s">
         <v>121</v>
       </c>
       <c r="C74" s="12"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A75" s="49" t="s">
+      <c r="A75" s="45" t="s">
         <v>122</v>
       </c>
-      <c r="B75" s="63" t="s">
+      <c r="B75" s="58" t="s">
         <v>123</v>
       </c>
       <c r="C75" s="12"/>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A76" s="49" t="s">
+      <c r="A76" s="45" t="s">
         <v>124</v>
       </c>
-      <c r="B76" s="63" t="s">
+      <c r="B76" s="58" t="s">
         <v>125</v>
       </c>
       <c r="C76" s="12"/>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A77" s="52" t="s">
+      <c r="A77" s="48" t="s">
         <v>126</v>
       </c>
-      <c r="B77" s="70" t="s">
+      <c r="B77" s="65" t="s">
         <v>127</v>
       </c>
       <c r="C77" s="12"/>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A78" s="49" t="s">
+      <c r="A78" s="45" t="s">
         <v>128</v>
       </c>
-      <c r="B78" s="63" t="s">
+      <c r="B78" s="58" t="s">
         <v>129</v>
       </c>
       <c r="C78" s="12"/>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A79" s="49" t="s">
+      <c r="A79" s="45" t="s">
         <v>130</v>
       </c>
-      <c r="B79" s="63" t="s">
+      <c r="B79" s="58" t="s">
         <v>131</v>
       </c>
       <c r="C79" s="12"/>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A80" s="49" t="s">
+      <c r="A80" s="45" t="s">
         <v>132</v>
       </c>
-      <c r="B80" s="63" t="s">
+      <c r="B80" s="58" t="s">
         <v>133</v>
       </c>
       <c r="C80" s="12"/>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A81" s="52" t="s">
+      <c r="A81" s="48" t="s">
         <v>134</v>
       </c>
-      <c r="B81" s="70" t="s">
+      <c r="B81" s="65" t="s">
         <v>135</v>
       </c>
       <c r="C81" s="12"/>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A82" s="49" t="s">
+      <c r="A82" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="B82" s="63" t="s">
+      <c r="B82" s="58" t="s">
         <v>137</v>
       </c>
       <c r="C82" s="12"/>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A83" s="49" t="s">
+      <c r="A83" s="45" t="s">
         <v>138</v>
       </c>
-      <c r="B83" s="63" t="s">
+      <c r="B83" s="58" t="s">
         <v>139</v>
       </c>
       <c r="C83" s="12"/>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A84" s="49" t="s">
+      <c r="A84" s="45" t="s">
         <v>140</v>
       </c>
-      <c r="B84" s="63" t="s">
+      <c r="B84" s="58" t="s">
         <v>141</v>
       </c>
       <c r="C84" s="12"/>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A85" s="52" t="s">
+      <c r="A85" s="48" t="s">
         <v>142</v>
       </c>
-      <c r="B85" s="70" t="s">
+      <c r="B85" s="65" t="s">
         <v>143</v>
       </c>
       <c r="C85" s="12"/>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A86" s="49" t="s">
+      <c r="A86" s="45" t="s">
         <v>144</v>
       </c>
-      <c r="B86" s="63" t="s">
+      <c r="B86" s="58" t="s">
         <v>145</v>
       </c>
       <c r="C86" s="12"/>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A87" s="49" t="s">
+      <c r="A87" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="B87" s="63" t="s">
+      <c r="B87" s="58" t="s">
         <v>147</v>
       </c>
       <c r="C87" s="12"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A88" s="49" t="s">
+      <c r="A88" s="45" t="s">
         <v>148</v>
       </c>
-      <c r="B88" s="63" t="s">
+      <c r="B88" s="58" t="s">
         <v>149</v>
       </c>
       <c r="C88" s="12"/>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A89" s="52" t="s">
+      <c r="A89" s="48" t="s">
         <v>150</v>
       </c>
-      <c r="B89" s="70" t="s">
+      <c r="B89" s="65" t="s">
         <v>151</v>
       </c>
       <c r="C89" s="12"/>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A90" s="49" t="s">
+      <c r="A90" s="45" t="s">
         <v>152</v>
       </c>
-      <c r="B90" s="63" t="s">
+      <c r="B90" s="58" t="s">
         <v>153</v>
       </c>
       <c r="C90" s="12"/>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A91" s="49" t="s">
+      <c r="A91" s="45" t="s">
         <v>154</v>
       </c>
-      <c r="B91" s="63" t="s">
+      <c r="B91" s="58" t="s">
         <v>155</v>
       </c>
       <c r="C91" s="12"/>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A92" s="49" t="s">
+      <c r="A92" s="45" t="s">
         <v>156</v>
       </c>
-      <c r="B92" s="63" t="s">
+      <c r="B92" s="58" t="s">
         <v>157</v>
       </c>
       <c r="C92" s="12"/>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A93" s="52" t="s">
+      <c r="A93" s="48" t="s">
         <v>158</v>
       </c>
-      <c r="B93" s="70" t="s">
+      <c r="B93" s="65" t="s">
         <v>159</v>
       </c>
       <c r="C93" s="12"/>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A94" s="49" t="s">
+      <c r="A94" s="45" t="s">
         <v>160</v>
       </c>
-      <c r="B94" s="63" t="s">
+      <c r="B94" s="58" t="s">
         <v>161</v>
       </c>
       <c r="C94" s="12"/>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A95" s="49" t="s">
+      <c r="A95" s="45" t="s">
         <v>162</v>
       </c>
-      <c r="B95" s="63" t="s">
+      <c r="B95" s="58" t="s">
         <v>163</v>
       </c>
       <c r="C95" s="12"/>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A96" s="49" t="s">
+      <c r="A96" s="45" t="s">
         <v>164</v>
       </c>
-      <c r="B96" s="63" t="s">
+      <c r="B96" s="58" t="s">
         <v>165</v>
       </c>
       <c r="C96" s="12"/>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A97" s="52" t="s">
+      <c r="A97" s="48" t="s">
         <v>166</v>
       </c>
-      <c r="B97" s="70" t="s">
+      <c r="B97" s="65" t="s">
         <v>167</v>
       </c>
       <c r="C97" s="12"/>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A98" s="49" t="s">
+      <c r="A98" s="45" t="s">
         <v>168</v>
       </c>
-      <c r="B98" s="63" t="s">
+      <c r="B98" s="58" t="s">
         <v>169</v>
       </c>
       <c r="C98" s="12"/>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A99" s="49" t="s">
+      <c r="A99" s="45" t="s">
         <v>170</v>
       </c>
-      <c r="B99" s="63" t="s">
+      <c r="B99" s="58" t="s">
         <v>171</v>
       </c>
       <c r="C99" s="12"/>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A100" s="49" t="s">
+      <c r="A100" s="45" t="s">
         <v>172</v>
       </c>
-      <c r="B100" s="63" t="s">
+      <c r="B100" s="58" t="s">
         <v>173</v>
       </c>
       <c r="C100" s="12"/>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A101" s="52" t="s">
+      <c r="A101" s="48" t="s">
         <v>174</v>
       </c>
-      <c r="B101" s="70" t="s">
+      <c r="B101" s="65" t="s">
         <v>175</v>
       </c>
       <c r="C101" s="12"/>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A102" s="49" t="s">
+      <c r="A102" s="45" t="s">
         <v>176</v>
       </c>
-      <c r="B102" s="63" t="s">
+      <c r="B102" s="58" t="s">
         <v>177</v>
       </c>
       <c r="C102" s="12"/>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A103" s="49" t="s">
+      <c r="A103" s="45" t="s">
         <v>178</v>
       </c>
-      <c r="B103" s="63" t="s">
+      <c r="B103" s="58" t="s">
         <v>179</v>
       </c>
       <c r="C103" s="12"/>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A104" s="49" t="s">
+      <c r="A104" s="45" t="s">
         <v>180</v>
       </c>
-      <c r="B104" s="63" t="s">
+      <c r="B104" s="58" t="s">
         <v>181</v>
       </c>
       <c r="C104" s="12"/>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A105" s="52" t="s">
+      <c r="A105" s="48" t="s">
         <v>182</v>
       </c>
-      <c r="B105" s="70" t="s">
+      <c r="B105" s="65" t="s">
         <v>183</v>
       </c>
       <c r="C105" s="12"/>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A106" s="49" t="s">
+      <c r="A106" s="45" t="s">
         <v>184</v>
       </c>
-      <c r="B106" s="63" t="s">
+      <c r="B106" s="58" t="s">
         <v>185</v>
       </c>
       <c r="C106" s="12"/>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A107" s="49" t="s">
+      <c r="A107" s="45" t="s">
         <v>186</v>
       </c>
-      <c r="B107" s="63" t="s">
+      <c r="B107" s="58" t="s">
         <v>187</v>
       </c>
       <c r="C107" s="12"/>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A108" s="49" t="s">
+      <c r="A108" s="45" t="s">
         <v>188</v>
       </c>
-      <c r="B108" s="63" t="s">
+      <c r="B108" s="58" t="s">
         <v>189</v>
       </c>
       <c r="C108" s="12"/>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A109" s="52" t="s">
+      <c r="A109" s="48" t="s">
         <v>190</v>
       </c>
-      <c r="B109" s="70" t="s">
+      <c r="B109" s="65" t="s">
         <v>191</v>
       </c>
       <c r="C109" s="12"/>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A110" s="49" t="s">
+      <c r="A110" s="45" t="s">
         <v>192</v>
       </c>
-      <c r="B110" s="63" t="s">
+      <c r="B110" s="58" t="s">
         <v>193</v>
       </c>
       <c r="C110" s="12"/>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A111" s="49" t="s">
+      <c r="A111" s="45" t="s">
         <v>194</v>
       </c>
-      <c r="B111" s="63" t="s">
+      <c r="B111" s="58" t="s">
         <v>195</v>
       </c>
       <c r="C111" s="12"/>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A112" s="49" t="s">
+      <c r="A112" s="45" t="s">
         <v>196</v>
       </c>
-      <c r="B112" s="63" t="s">
+      <c r="B112" s="58" t="s">
         <v>197</v>
       </c>
       <c r="C112" s="12"/>
     </row>
     <row r="113" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="50" t="s">
+      <c r="A113" s="46" t="s">
         <v>198</v>
       </c>
-      <c r="B113" s="69" t="s">
+      <c r="B113" s="64" t="s">
         <v>199</v>
       </c>
       <c r="C113" s="12"/>
     </row>
     <row r="114" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="51"/>
-      <c r="B114" s="64" t="s">
+      <c r="A114" s="47"/>
+      <c r="B114" s="59" t="s">
         <v>221</v>
       </c>
       <c r="C114" s="15"/>

</xml_diff>

<commit_message>
Small Change in template and prepation for business data config
</commit_message>
<xml_diff>
--- a/HkwgConverter/Sample/Template_Kiss_Input.xlsx
+++ b/HkwgConverter/Sample/Template_Kiss_Input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="28515" windowHeight="15135" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="20730" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="3" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="224">
   <si>
     <t>Info</t>
   </si>
@@ -685,6 +685,9 @@
   </si>
   <si>
     <t>Extern</t>
+  </si>
+  <si>
+    <t>Intraday-FLEX</t>
   </si>
 </sst>
 </file>
@@ -1556,7 +1559,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1583,7 +1586,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="24" t="s">
-        <v>206</v>
+        <v>223</v>
       </c>
       <c r="B2" s="26" t="s">
         <v>208</v>

</xml_diff>